<commit_message>
Nwe data for power group 1 and 2
</commit_message>
<xml_diff>
--- a/DataSet_VersionRecuperada.xlsx
+++ b/DataSet_VersionRecuperada.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UDEA-MAESTRIA\Proyecto\Resultados\Sujetos Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UDEA-MAESTRIA\Thesis result\Data analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Group 1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="181">
   <si>
     <t>7:00 a 8:00</t>
   </si>
@@ -657,6 +657,9 @@
   <si>
     <t>Lado del daño</t>
   </si>
+  <si>
+    <t>Group 1 + Group 2</t>
+  </si>
 </sst>
 </file>
 
@@ -760,7 +763,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +833,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1105,15 +1114,6 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,10 +1126,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1139,6 +1142,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1181,6 +1190,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1466,10 +1481,10 @@
   <dimension ref="A1:AV26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:H19"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6254,9 +6269,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC249"/>
+  <dimension ref="A1:AR249"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="P1" sqref="P1:AC39"/>
     </sheetView>
   </sheetViews>
@@ -6281,100 +6296,153 @@
     <col min="25" max="25" width="2.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="2.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="27" max="29" width="4.5703125" style="33" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="11.42578125" style="5"/>
+    <col min="30" max="30" width="11.42578125" style="5"/>
+    <col min="31" max="31" width="9.7109375" style="5" customWidth="1"/>
+    <col min="32" max="32" width="2" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="2.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="2.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="4" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="68"/>
-      <c r="P1" s="66" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="66"/>
+      <c r="P1" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="68"/>
-    </row>
-    <row r="2" spans="1:29" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="66"/>
+      <c r="AE1" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="66"/>
+    </row>
+    <row r="2" spans="1:44" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="66" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="66" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
       <c r="L2" s="69" t="s">
         <v>128</v>
       </c>
       <c r="M2" s="70"/>
       <c r="N2" s="71"/>
-      <c r="P2" s="64" t="s">
+      <c r="P2" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="R2" s="66" t="s">
+      <c r="R2" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S2" s="67"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="66" t="s">
+      <c r="S2" s="65"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="67"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="66" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="68"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="66"/>
       <c r="AA2" s="69" t="s">
         <v>128</v>
       </c>
       <c r="AB2" s="70"/>
       <c r="AC2" s="71"/>
-    </row>
-    <row r="3" spans="1:29" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
+      <c r="AE2" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF2" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG2" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AJ2" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="71"/>
+    </row>
+    <row r="3" spans="1:44" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
       <c r="C3" s="36" t="s">
         <v>125</v>
       </c>
@@ -6411,8 +6479,8 @@
       <c r="N3" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
       <c r="R3" s="36" t="s">
         <v>125</v>
       </c>
@@ -6449,9 +6517,47 @@
       <c r="AC3" s="37" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP3" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ3" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR3" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="38" t="s">
@@ -6490,7 +6596,7 @@
       <c r="O4" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="P4" s="60" t="s">
+      <c r="P4" s="57" t="s">
         <v>136</v>
       </c>
       <c r="Q4" s="38" t="s">
@@ -6526,9 +6632,27 @@
       <c r="AC4" s="40">
         <v>0.80864800000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
+      <c r="AE4" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF4" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="39"/>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="39"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="40"/>
+      <c r="AQ4" s="40"/>
+      <c r="AR4" s="40"/>
+    </row>
+    <row r="5" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
       <c r="B5" s="38" t="s">
         <v>133</v>
       </c>
@@ -6550,13 +6674,13 @@
       <c r="H5" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" s="39" t="s">
+      <c r="I5" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="84" t="s">
         <v>108</v>
       </c>
       <c r="L5" s="40">
@@ -6568,7 +6692,7 @@
       <c r="N5" s="40">
         <v>0.53922099999999995</v>
       </c>
-      <c r="P5" s="61"/>
+      <c r="P5" s="58"/>
       <c r="Q5" s="38" t="s">
         <v>133</v>
       </c>
@@ -6590,13 +6714,13 @@
       <c r="W5" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X5" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y5" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z5" s="39" t="s">
+      <c r="X5" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y5" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" s="84" t="s">
         <v>108</v>
       </c>
       <c r="AA5" s="40">
@@ -6608,9 +6732,25 @@
       <c r="AC5" s="40">
         <v>0.74212500000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="39"/>
+      <c r="AI5" s="39"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="39"/>
+      <c r="AL5" s="39"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="39"/>
+      <c r="AO5" s="39"/>
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
+    </row>
+    <row r="6" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
       <c r="B6" s="38" t="s">
         <v>134</v>
       </c>
@@ -6646,7 +6786,7 @@
       <c r="N6" s="40">
         <v>4.9845799999999997E-3</v>
       </c>
-      <c r="P6" s="61"/>
+      <c r="P6" s="58"/>
       <c r="Q6" s="38" t="s">
         <v>134</v>
       </c>
@@ -6680,9 +6820,25 @@
       <c r="AC6" s="40">
         <v>0.32851900000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="38"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="39"/>
+      <c r="AP6" s="40"/>
+      <c r="AQ6" s="40"/>
+      <c r="AR6" s="40"/>
+    </row>
+    <row r="7" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
       <c r="B7" s="41" t="s">
         <v>135</v>
       </c>
@@ -6704,7 +6860,7 @@
       <c r="N7" s="42">
         <v>6.9331199999999996E-4</v>
       </c>
-      <c r="P7" s="62"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="41" t="s">
         <v>135</v>
       </c>
@@ -6726,9 +6882,25 @@
       <c r="AC7" s="42">
         <v>5.0963000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG7" s="41"/>
+      <c r="AH7" s="41"/>
+      <c r="AI7" s="41"/>
+      <c r="AJ7" s="41"/>
+      <c r="AK7" s="41"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="42"/>
+      <c r="AQ7" s="42"/>
+      <c r="AR7" s="42"/>
+    </row>
+    <row r="8" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
         <v>137</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -6764,7 +6936,7 @@
       <c r="N8" s="40">
         <v>0.34474100000000002</v>
       </c>
-      <c r="P8" s="60" t="s">
+      <c r="P8" s="57" t="s">
         <v>137</v>
       </c>
       <c r="Q8" s="38" t="s">
@@ -6800,9 +6972,27 @@
       <c r="AC8" s="40">
         <v>0.83276700000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="AE8" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF8" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="39"/>
+      <c r="AJ8" s="38"/>
+      <c r="AK8" s="38"/>
+      <c r="AL8" s="39"/>
+      <c r="AM8" s="38"/>
+      <c r="AN8" s="38"/>
+      <c r="AO8" s="38"/>
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40"/>
+      <c r="AR8" s="40"/>
+    </row>
+    <row r="9" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
       <c r="B9" s="38" t="s">
         <v>133</v>
       </c>
@@ -6824,13 +7014,13 @@
       <c r="H9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="39" t="s">
+      <c r="I9" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="84" t="s">
         <v>108</v>
       </c>
       <c r="L9" s="40">
@@ -6842,7 +7032,7 @@
       <c r="N9" s="40">
         <v>0.93847400000000003</v>
       </c>
-      <c r="P9" s="61"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="38" t="s">
         <v>133</v>
       </c>
@@ -6864,13 +7054,13 @@
       <c r="W9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X9" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y9" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z9" s="39" t="s">
+      <c r="X9" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y9" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z9" s="84" t="s">
         <v>108</v>
       </c>
       <c r="AA9" s="40">
@@ -6882,9 +7072,25 @@
       <c r="AC9" s="40">
         <v>0.36027500000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="AE9" s="58"/>
+      <c r="AF9" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="39"/>
+      <c r="AJ9" s="38"/>
+      <c r="AK9" s="38"/>
+      <c r="AL9" s="39"/>
+      <c r="AM9" s="38"/>
+      <c r="AN9" s="38"/>
+      <c r="AO9" s="39"/>
+      <c r="AP9" s="40"/>
+      <c r="AQ9" s="40"/>
+      <c r="AR9" s="40"/>
+    </row>
+    <row r="10" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
       <c r="B10" s="38" t="s">
         <v>134</v>
       </c>
@@ -6920,7 +7126,7 @@
       <c r="N10" s="40">
         <v>1.1750500000000001E-2</v>
       </c>
-      <c r="P10" s="61"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="38" t="s">
         <v>134</v>
       </c>
@@ -6954,9 +7160,25 @@
       <c r="AC10" s="40">
         <v>0.42157099999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="AE10" s="58"/>
+      <c r="AF10" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="39"/>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="38"/>
+      <c r="AL10" s="39"/>
+      <c r="AM10" s="38"/>
+      <c r="AN10" s="38"/>
+      <c r="AO10" s="39"/>
+      <c r="AP10" s="40"/>
+      <c r="AQ10" s="40"/>
+      <c r="AR10" s="40"/>
+    </row>
+    <row r="11" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="41" t="s">
         <v>135</v>
       </c>
@@ -6978,7 +7200,7 @@
       <c r="N11" s="42">
         <v>4.1270400000000002E-3</v>
       </c>
-      <c r="P11" s="62"/>
+      <c r="P11" s="59"/>
       <c r="Q11" s="41" t="s">
         <v>135</v>
       </c>
@@ -7006,9 +7228,25 @@
       <c r="AC11" s="42">
         <v>8.3578299999999994E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG11" s="41"/>
+      <c r="AH11" s="41"/>
+      <c r="AI11" s="41"/>
+      <c r="AJ11" s="41"/>
+      <c r="AK11" s="41"/>
+      <c r="AL11" s="41"/>
+      <c r="AM11" s="41"/>
+      <c r="AN11" s="41"/>
+      <c r="AO11" s="41"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="42"/>
+      <c r="AR11" s="42"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="38" t="s">
@@ -7044,7 +7282,7 @@
       <c r="N12" s="40">
         <v>0.61764799999999997</v>
       </c>
-      <c r="P12" s="60" t="s">
+      <c r="P12" s="57" t="s">
         <v>110</v>
       </c>
       <c r="Q12" s="38" t="s">
@@ -7080,9 +7318,27 @@
       <c r="AC12" s="40">
         <v>0.72725300000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="AE12" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF12" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="39"/>
+      <c r="AI12" s="38"/>
+      <c r="AJ12" s="38"/>
+      <c r="AK12" s="39"/>
+      <c r="AL12" s="38"/>
+      <c r="AM12" s="38"/>
+      <c r="AN12" s="39"/>
+      <c r="AO12" s="38"/>
+      <c r="AP12" s="40"/>
+      <c r="AQ12" s="40"/>
+      <c r="AR12" s="40"/>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
       <c r="B13" s="38" t="s">
         <v>133</v>
       </c>
@@ -7116,7 +7372,7 @@
       <c r="N13" s="40">
         <v>0.18202299999999999</v>
       </c>
-      <c r="P13" s="61"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="38" t="s">
         <v>133</v>
       </c>
@@ -7150,9 +7406,25 @@
       <c r="AC13" s="40">
         <v>0.50264500000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="AE13" s="58"/>
+      <c r="AF13" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="39"/>
+      <c r="AI13" s="39"/>
+      <c r="AJ13" s="38"/>
+      <c r="AK13" s="39"/>
+      <c r="AL13" s="39"/>
+      <c r="AM13" s="38"/>
+      <c r="AN13" s="39"/>
+      <c r="AO13" s="39"/>
+      <c r="AP13" s="40"/>
+      <c r="AQ13" s="40"/>
+      <c r="AR13" s="40"/>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
       <c r="B14" s="38" t="s">
         <v>134</v>
       </c>
@@ -7186,7 +7458,7 @@
       <c r="N14" s="40">
         <v>5.4985399999999997E-2</v>
       </c>
-      <c r="P14" s="61"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="38" t="s">
         <v>134</v>
       </c>
@@ -7220,9 +7492,25 @@
       <c r="AC14" s="40">
         <v>0.35624899999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="39"/>
+      <c r="AI14" s="39"/>
+      <c r="AJ14" s="38"/>
+      <c r="AK14" s="39"/>
+      <c r="AL14" s="39"/>
+      <c r="AM14" s="38"/>
+      <c r="AN14" s="39"/>
+      <c r="AO14" s="39"/>
+      <c r="AP14" s="40"/>
+      <c r="AQ14" s="40"/>
+      <c r="AR14" s="40"/>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
       <c r="B15" s="41" t="s">
         <v>135</v>
       </c>
@@ -7244,7 +7532,7 @@
       <c r="N15" s="42">
         <v>0</v>
       </c>
-      <c r="P15" s="62"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="41" t="s">
         <v>135</v>
       </c>
@@ -7272,9 +7560,25 @@
       <c r="AC15" s="42">
         <v>0.228573</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="AE15" s="59"/>
+      <c r="AF15" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG15" s="41"/>
+      <c r="AH15" s="41"/>
+      <c r="AI15" s="41"/>
+      <c r="AJ15" s="41"/>
+      <c r="AK15" s="41"/>
+      <c r="AL15" s="41"/>
+      <c r="AM15" s="41"/>
+      <c r="AN15" s="41"/>
+      <c r="AO15" s="41"/>
+      <c r="AP15" s="42"/>
+      <c r="AQ15" s="42"/>
+      <c r="AR15" s="42"/>
+    </row>
+    <row r="16" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="39" t="s">
@@ -7298,7 +7602,7 @@
       <c r="H16" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="83" t="s">
         <v>108</v>
       </c>
       <c r="J16" s="39"/>
@@ -7312,7 +7616,7 @@
       <c r="N16" s="40">
         <v>0.29320299999999999</v>
       </c>
-      <c r="P16" s="57" t="s">
+      <c r="P16" s="61" t="s">
         <v>138</v>
       </c>
       <c r="Q16" s="39" t="s">
@@ -7336,7 +7640,7 @@
       <c r="W16" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X16" s="38" t="s">
+      <c r="X16" s="83" t="s">
         <v>108</v>
       </c>
       <c r="Y16" s="39" t="s">
@@ -7352,9 +7656,51 @@
       <c r="AC16" s="40">
         <v>0.81892100000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="AE16" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF16" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG16" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ16" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM16" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO16" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP16" s="40">
+        <v>0.23941899999999999</v>
+      </c>
+      <c r="AQ16" s="40">
+        <v>0.23985999999999999</v>
+      </c>
+      <c r="AR16" s="40">
+        <v>6.7111699999999996E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
       <c r="B17" s="39" t="s">
         <v>133</v>
       </c>
@@ -7388,7 +7734,7 @@
       <c r="N17" s="40">
         <v>0.174321</v>
       </c>
-      <c r="P17" s="58"/>
+      <c r="P17" s="62"/>
       <c r="Q17" s="39" t="s">
         <v>133</v>
       </c>
@@ -7422,9 +7768,47 @@
       <c r="AC17" s="40">
         <v>0.46240999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
+      <c r="AE17" s="62"/>
+      <c r="AF17" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG17" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ17" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM17" s="38"/>
+      <c r="AN17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP17" s="40">
+        <v>8.2246399999999997E-2</v>
+      </c>
+      <c r="AQ17" s="40">
+        <v>6.4230999999999996E-2</v>
+      </c>
+      <c r="AR17" s="40">
+        <v>0.28881299999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="62"/>
       <c r="B18" s="38" t="s">
         <v>134</v>
       </c>
@@ -7462,7 +7846,7 @@
       <c r="N18" s="40">
         <v>1.3136500000000001E-2</v>
       </c>
-      <c r="P18" s="58"/>
+      <c r="P18" s="62"/>
       <c r="Q18" s="38" t="s">
         <v>134</v>
       </c>
@@ -7496,9 +7880,49 @@
       <c r="AC18" s="40">
         <v>0.97048199999999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
+      <c r="AE18" s="62"/>
+      <c r="AF18" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO18" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP18" s="40">
+        <v>0.55319600000000002</v>
+      </c>
+      <c r="AQ18" s="40">
+        <v>0.13298599999999999</v>
+      </c>
+      <c r="AR18" s="40">
+        <v>6.7111699999999996E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="63"/>
       <c r="B19" s="41" t="s">
         <v>135</v>
       </c>
@@ -7520,7 +7944,7 @@
       <c r="N19" s="42">
         <v>3.6087900000000002E-3</v>
       </c>
-      <c r="P19" s="59"/>
+      <c r="P19" s="63"/>
       <c r="Q19" s="41" t="s">
         <v>135</v>
       </c>
@@ -7550,9 +7974,35 @@
       <c r="AC19" s="42">
         <v>0.75703299999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="AE19" s="63"/>
+      <c r="AF19" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG19" s="41"/>
+      <c r="AH19" s="41"/>
+      <c r="AI19" s="41"/>
+      <c r="AJ19" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK19" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL19" s="41"/>
+      <c r="AM19" s="41"/>
+      <c r="AN19" s="41"/>
+      <c r="AO19" s="41"/>
+      <c r="AP19" s="42">
+        <v>2.3891699999999998E-2</v>
+      </c>
+      <c r="AQ19" s="42">
+        <v>0.26253700000000002</v>
+      </c>
+      <c r="AR19" s="42">
+        <v>1.8078400000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
         <v>139</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -7588,7 +8038,7 @@
       <c r="N20" s="40">
         <v>5.4854E-2</v>
       </c>
-      <c r="P20" s="57" t="s">
+      <c r="P20" s="61" t="s">
         <v>139</v>
       </c>
       <c r="Q20" s="38" t="s">
@@ -7624,9 +8074,45 @@
       <c r="AC20" s="40">
         <v>0.97633400000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="AE20" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF20" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG20" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH20" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI20" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ20" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK20" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL20" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM20" s="38"/>
+      <c r="AN20" s="39"/>
+      <c r="AO20" s="39"/>
+      <c r="AP20" s="40">
+        <v>0.11039</v>
+      </c>
+      <c r="AQ20" s="40">
+        <v>0.16622200000000001</v>
+      </c>
+      <c r="AR20" s="40">
+        <v>0.14690500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A21" s="62"/>
       <c r="B21" s="38" t="s">
         <v>133</v>
       </c>
@@ -7664,7 +8150,7 @@
       <c r="N21" s="40">
         <v>0.40772999999999998</v>
       </c>
-      <c r="P21" s="58"/>
+      <c r="P21" s="62"/>
       <c r="Q21" s="38" t="s">
         <v>133</v>
       </c>
@@ -7698,9 +8184,45 @@
       <c r="AC21" s="40">
         <v>0.34917199999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
+      <c r="AE21" s="62"/>
+      <c r="AF21" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG21" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH21" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI21" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ21" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK21" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL21" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM21" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AP21" s="40">
+        <v>9.6229999999999996E-2</v>
+      </c>
+      <c r="AQ21" s="40">
+        <v>3.94218E-2</v>
+      </c>
+      <c r="AR21" s="40">
+        <v>7.7744599999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A22" s="62"/>
       <c r="B22" s="38" t="s">
         <v>134</v>
       </c>
@@ -7734,7 +8256,7 @@
       <c r="N22" s="40">
         <v>5.7199100000000003E-2</v>
       </c>
-      <c r="P22" s="58"/>
+      <c r="P22" s="62"/>
       <c r="Q22" s="38" t="s">
         <v>134</v>
       </c>
@@ -7768,9 +8290,45 @@
       <c r="AC22" s="40">
         <v>0.98668299999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
+      <c r="AE22" s="62"/>
+      <c r="AF22" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG22" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH22" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI22" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ22" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK22" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL22" s="39"/>
+      <c r="AM22" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN22" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO22" s="39"/>
+      <c r="AP22" s="40">
+        <v>0.14286699999999999</v>
+      </c>
+      <c r="AQ22" s="40">
+        <v>1.6366600000000001E-3</v>
+      </c>
+      <c r="AR22" s="40">
+        <v>0.214117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A23" s="63"/>
       <c r="B23" s="41" t="s">
         <v>135</v>
       </c>
@@ -7792,7 +8350,7 @@
       <c r="N23" s="42">
         <v>7.4505699999999994E-2</v>
       </c>
-      <c r="P23" s="59"/>
+      <c r="P23" s="63"/>
       <c r="Q23" s="41" t="s">
         <v>135</v>
       </c>
@@ -7822,9 +8380,35 @@
       <c r="AC23" s="42">
         <v>0.96269300000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
+      <c r="AE23" s="63"/>
+      <c r="AF23" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG23" s="41"/>
+      <c r="AH23" s="41"/>
+      <c r="AI23" s="41"/>
+      <c r="AJ23" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK23" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL23" s="41"/>
+      <c r="AM23" s="41"/>
+      <c r="AN23" s="41"/>
+      <c r="AO23" s="41"/>
+      <c r="AP23" s="42">
+        <v>1.78631E-2</v>
+      </c>
+      <c r="AQ23" s="42">
+        <v>1.0533300000000001E-2</v>
+      </c>
+      <c r="AR23" s="42">
+        <v>0.190696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
         <v>140</v>
       </c>
       <c r="B24" s="38" t="s">
@@ -7866,7 +8450,7 @@
       <c r="N24" s="40">
         <v>0.25895099999999999</v>
       </c>
-      <c r="P24" s="60" t="s">
+      <c r="P24" s="57" t="s">
         <v>140</v>
       </c>
       <c r="Q24" s="38" t="s">
@@ -7902,9 +8486,49 @@
       <c r="AC24" s="40">
         <v>0.391177</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="AE24" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF24" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG24" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ24" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM24" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO24" s="39"/>
+      <c r="AP24" s="40">
+        <v>2.0717699999999999E-2</v>
+      </c>
+      <c r="AQ24" s="40">
+        <v>2.11925E-2</v>
+      </c>
+      <c r="AR24" s="40">
+        <v>7.4277599999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
       <c r="B25" s="38" t="s">
         <v>133</v>
       </c>
@@ -7938,7 +8562,7 @@
       <c r="N25" s="40">
         <v>8.7913599999999995E-2</v>
       </c>
-      <c r="P25" s="61"/>
+      <c r="P25" s="58"/>
       <c r="Q25" s="38" t="s">
         <v>133</v>
       </c>
@@ -7972,9 +8596,43 @@
       <c r="AC25" s="40">
         <v>0.992869</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="AE25" s="58"/>
+      <c r="AF25" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG25" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ25" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM25" s="38"/>
+      <c r="AN25" s="39"/>
+      <c r="AO25" s="39"/>
+      <c r="AP25" s="40">
+        <v>0.24904799999999999</v>
+      </c>
+      <c r="AQ25" s="40">
+        <v>0.58647499999999997</v>
+      </c>
+      <c r="AR25" s="40">
+        <v>0.16930899999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
       <c r="B26" s="38" t="s">
         <v>134</v>
       </c>
@@ -8010,7 +8668,7 @@
       <c r="N26" s="40">
         <v>8.6047599999999999E-5</v>
       </c>
-      <c r="P26" s="61"/>
+      <c r="P26" s="58"/>
       <c r="Q26" s="38" t="s">
         <v>134</v>
       </c>
@@ -8046,9 +8704,47 @@
       <c r="AC26" s="40">
         <v>0.49700499999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
+      <c r="AE26" s="58"/>
+      <c r="AF26" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG26" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ26" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM26" s="38"/>
+      <c r="AN26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO26" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP26" s="40">
+        <v>5.1557899999999997E-2</v>
+      </c>
+      <c r="AQ26" s="40">
+        <v>0.182893</v>
+      </c>
+      <c r="AR26" s="40">
+        <v>9.6222600000000005E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
       <c r="B27" s="41" t="s">
         <v>135</v>
       </c>
@@ -8070,7 +8766,7 @@
       <c r="N27" s="42">
         <v>5.1660999999999999E-2</v>
       </c>
-      <c r="P27" s="62"/>
+      <c r="P27" s="59"/>
       <c r="Q27" s="41" t="s">
         <v>135</v>
       </c>
@@ -8098,9 +8794,33 @@
       <c r="AC27" s="42">
         <v>0.59972999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
+      <c r="AE27" s="59"/>
+      <c r="AF27" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG27" s="41"/>
+      <c r="AH27" s="41"/>
+      <c r="AI27" s="41"/>
+      <c r="AJ27" s="41"/>
+      <c r="AK27" s="41"/>
+      <c r="AL27" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM27" s="41"/>
+      <c r="AN27" s="41"/>
+      <c r="AO27" s="41"/>
+      <c r="AP27" s="42">
+        <v>5.3174899999999997E-2</v>
+      </c>
+      <c r="AQ27" s="42">
+        <v>7.1961000000000004E-3</v>
+      </c>
+      <c r="AR27" s="42">
+        <v>2.1038399999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>116</v>
       </c>
       <c r="B28" s="38" t="s">
@@ -8136,7 +8856,7 @@
       <c r="N28" s="40">
         <v>0.21804599999999999</v>
       </c>
-      <c r="P28" s="60" t="s">
+      <c r="P28" s="57" t="s">
         <v>116</v>
       </c>
       <c r="Q28" s="38" t="s">
@@ -8172,9 +8892,27 @@
       <c r="AC28" s="40">
         <v>0.79758499999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="AE28" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF28" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG28" s="38"/>
+      <c r="AH28" s="39"/>
+      <c r="AI28" s="39"/>
+      <c r="AJ28" s="38"/>
+      <c r="AK28" s="39"/>
+      <c r="AL28" s="39"/>
+      <c r="AM28" s="38"/>
+      <c r="AN28" s="39"/>
+      <c r="AO28" s="39"/>
+      <c r="AP28" s="40"/>
+      <c r="AQ28" s="40"/>
+      <c r="AR28" s="40"/>
+    </row>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A29" s="58"/>
       <c r="B29" s="38" t="s">
         <v>133</v>
       </c>
@@ -8208,7 +8946,7 @@
       <c r="N29" s="40">
         <v>1.9599700000000001E-2</v>
       </c>
-      <c r="P29" s="61"/>
+      <c r="P29" s="58"/>
       <c r="Q29" s="38" t="s">
         <v>133</v>
       </c>
@@ -8242,9 +8980,25 @@
       <c r="AC29" s="40">
         <v>0.20802399999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="AE29" s="58"/>
+      <c r="AF29" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG29" s="38"/>
+      <c r="AH29" s="39"/>
+      <c r="AI29" s="39"/>
+      <c r="AJ29" s="38"/>
+      <c r="AK29" s="39"/>
+      <c r="AL29" s="39"/>
+      <c r="AM29" s="38"/>
+      <c r="AN29" s="39"/>
+      <c r="AO29" s="39"/>
+      <c r="AP29" s="40"/>
+      <c r="AQ29" s="40"/>
+      <c r="AR29" s="40"/>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
       <c r="B30" s="38" t="s">
         <v>134</v>
       </c>
@@ -8278,7 +9032,7 @@
       <c r="N30" s="40">
         <v>7.6017100000000002E-4</v>
       </c>
-      <c r="P30" s="61"/>
+      <c r="P30" s="58"/>
       <c r="Q30" s="38" t="s">
         <v>134</v>
       </c>
@@ -8312,9 +9066,25 @@
       <c r="AC30" s="40">
         <v>0.55451899999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
+      <c r="AE30" s="58"/>
+      <c r="AF30" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="39"/>
+      <c r="AI30" s="39"/>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="39"/>
+      <c r="AL30" s="39"/>
+      <c r="AM30" s="38"/>
+      <c r="AN30" s="39"/>
+      <c r="AO30" s="39"/>
+      <c r="AP30" s="40"/>
+      <c r="AQ30" s="40"/>
+      <c r="AR30" s="40"/>
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
       <c r="B31" s="41" t="s">
         <v>135</v>
       </c>
@@ -8336,7 +9106,7 @@
       <c r="N31" s="42">
         <v>6.0392800000000003E-2</v>
       </c>
-      <c r="P31" s="62"/>
+      <c r="P31" s="59"/>
       <c r="Q31" s="41" t="s">
         <v>135</v>
       </c>
@@ -8364,9 +9134,25 @@
       <c r="AC31" s="42">
         <v>0.40330300000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="60" t="s">
+      <c r="AE31" s="59"/>
+      <c r="AF31" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG31" s="41"/>
+      <c r="AH31" s="41"/>
+      <c r="AI31" s="41"/>
+      <c r="AJ31" s="41"/>
+      <c r="AK31" s="41"/>
+      <c r="AL31" s="41"/>
+      <c r="AM31" s="41"/>
+      <c r="AN31" s="41"/>
+      <c r="AO31" s="41"/>
+      <c r="AP31" s="42"/>
+      <c r="AQ31" s="42"/>
+      <c r="AR31" s="42"/>
+    </row>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
         <v>141</v>
       </c>
       <c r="B32" s="38" t="s">
@@ -8406,7 +9192,7 @@
       <c r="N32" s="40">
         <v>6.8416699999999997E-2</v>
       </c>
-      <c r="P32" s="60" t="s">
+      <c r="P32" s="57" t="s">
         <v>141</v>
       </c>
       <c r="Q32" s="38" t="s">
@@ -8442,9 +9228,27 @@
       <c r="AC32" s="40">
         <v>0.79306100000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="AE32" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF32" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG32" s="38"/>
+      <c r="AH32" s="39"/>
+      <c r="AI32" s="39"/>
+      <c r="AJ32" s="38"/>
+      <c r="AK32" s="39"/>
+      <c r="AL32" s="39"/>
+      <c r="AM32" s="38"/>
+      <c r="AN32" s="39"/>
+      <c r="AO32" s="39"/>
+      <c r="AP32" s="40"/>
+      <c r="AQ32" s="40"/>
+      <c r="AR32" s="40"/>
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A33" s="58"/>
       <c r="B33" s="38" t="s">
         <v>133</v>
       </c>
@@ -8478,7 +9282,7 @@
       <c r="N33" s="40">
         <v>0.24232799999999999</v>
       </c>
-      <c r="P33" s="61"/>
+      <c r="P33" s="58"/>
       <c r="Q33" s="38" t="s">
         <v>133</v>
       </c>
@@ -8512,9 +9316,25 @@
       <c r="AC33" s="40">
         <v>0.79171599999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="AE33" s="58"/>
+      <c r="AF33" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG33" s="38"/>
+      <c r="AH33" s="39"/>
+      <c r="AI33" s="39"/>
+      <c r="AJ33" s="38"/>
+      <c r="AK33" s="39"/>
+      <c r="AL33" s="39"/>
+      <c r="AM33" s="38"/>
+      <c r="AN33" s="39"/>
+      <c r="AO33" s="39"/>
+      <c r="AP33" s="40"/>
+      <c r="AQ33" s="40"/>
+      <c r="AR33" s="40"/>
+    </row>
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A34" s="58"/>
       <c r="B34" s="38" t="s">
         <v>134</v>
       </c>
@@ -8548,7 +9368,7 @@
       <c r="N34" s="40">
         <v>9.2139299999999993E-2</v>
       </c>
-      <c r="P34" s="61"/>
+      <c r="P34" s="58"/>
       <c r="Q34" s="38" t="s">
         <v>134</v>
       </c>
@@ -8584,9 +9404,25 @@
       <c r="AC34" s="40">
         <v>5.10708E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
+      <c r="AE34" s="58"/>
+      <c r="AF34" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG34" s="38"/>
+      <c r="AH34" s="39"/>
+      <c r="AI34" s="39"/>
+      <c r="AJ34" s="38"/>
+      <c r="AK34" s="39"/>
+      <c r="AL34" s="39"/>
+      <c r="AM34" s="38"/>
+      <c r="AN34" s="39"/>
+      <c r="AO34" s="39"/>
+      <c r="AP34" s="40"/>
+      <c r="AQ34" s="40"/>
+      <c r="AR34" s="40"/>
+    </row>
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A35" s="59"/>
       <c r="B35" s="41" t="s">
         <v>135</v>
       </c>
@@ -8608,7 +9444,7 @@
       <c r="N35" s="42">
         <v>3.5705899999999999E-2</v>
       </c>
-      <c r="P35" s="62"/>
+      <c r="P35" s="59"/>
       <c r="Q35" s="41" t="s">
         <v>135</v>
       </c>
@@ -8640,9 +9476,25 @@
       <c r="AC35" s="42">
         <v>0.37054599999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="AE35" s="59"/>
+      <c r="AF35" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG35" s="41"/>
+      <c r="AH35" s="41"/>
+      <c r="AI35" s="41"/>
+      <c r="AJ35" s="41"/>
+      <c r="AK35" s="41"/>
+      <c r="AL35" s="41"/>
+      <c r="AM35" s="41"/>
+      <c r="AN35" s="41"/>
+      <c r="AO35" s="41"/>
+      <c r="AP35" s="42"/>
+      <c r="AQ35" s="42"/>
+      <c r="AR35" s="42"/>
+    </row>
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A36" s="60" t="s">
         <v>142</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -8684,7 +9536,7 @@
       <c r="N36" s="40">
         <v>0.79885600000000001</v>
       </c>
-      <c r="P36" s="63" t="s">
+      <c r="P36" s="60" t="s">
         <v>142</v>
       </c>
       <c r="Q36" s="38" t="s">
@@ -8720,9 +9572,27 @@
       <c r="AC36" s="40">
         <v>0.119131</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="63"/>
+      <c r="AE36" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF36" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG36" s="38"/>
+      <c r="AH36" s="39"/>
+      <c r="AI36" s="39"/>
+      <c r="AJ36" s="38"/>
+      <c r="AK36" s="39"/>
+      <c r="AL36" s="39"/>
+      <c r="AM36" s="38"/>
+      <c r="AN36" s="39"/>
+      <c r="AO36" s="39"/>
+      <c r="AP36" s="40"/>
+      <c r="AQ36" s="40"/>
+      <c r="AR36" s="40"/>
+    </row>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A37" s="60"/>
       <c r="B37" s="38" t="s">
         <v>133</v>
       </c>
@@ -8756,7 +9626,7 @@
       <c r="N37" s="40">
         <v>0.51789499999999999</v>
       </c>
-      <c r="P37" s="63"/>
+      <c r="P37" s="60"/>
       <c r="Q37" s="38" t="s">
         <v>133</v>
       </c>
@@ -8790,9 +9660,25 @@
       <c r="AC37" s="40">
         <v>0.74060099999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="63"/>
+      <c r="AE37" s="60"/>
+      <c r="AF37" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG37" s="38"/>
+      <c r="AH37" s="39"/>
+      <c r="AI37" s="39"/>
+      <c r="AJ37" s="38"/>
+      <c r="AK37" s="39"/>
+      <c r="AL37" s="39"/>
+      <c r="AM37" s="38"/>
+      <c r="AN37" s="39"/>
+      <c r="AO37" s="39"/>
+      <c r="AP37" s="40"/>
+      <c r="AQ37" s="40"/>
+      <c r="AR37" s="40"/>
+    </row>
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
       <c r="B38" s="38" t="s">
         <v>134</v>
       </c>
@@ -8814,13 +9700,13 @@
       <c r="H38" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="J38" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="K38" s="39" t="s">
+      <c r="I38" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="K38" s="84" t="s">
         <v>108</v>
       </c>
       <c r="L38" s="40">
@@ -8832,7 +9718,7 @@
       <c r="N38" s="40">
         <v>1.3228699999999999E-2</v>
       </c>
-      <c r="P38" s="63"/>
+      <c r="P38" s="60"/>
       <c r="Q38" s="38" t="s">
         <v>134</v>
       </c>
@@ -8854,13 +9740,13 @@
       <c r="W38" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X38" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y38" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z38" s="39" t="s">
+      <c r="X38" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y38" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z38" s="84" t="s">
         <v>108</v>
       </c>
       <c r="AA38" s="40">
@@ -8872,9 +9758,25 @@
       <c r="AC38" s="40">
         <v>0.59381899999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="63"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG38" s="38"/>
+      <c r="AH38" s="39"/>
+      <c r="AI38" s="39"/>
+      <c r="AJ38" s="38"/>
+      <c r="AK38" s="39"/>
+      <c r="AL38" s="39"/>
+      <c r="AM38" s="38"/>
+      <c r="AN38" s="39"/>
+      <c r="AO38" s="39"/>
+      <c r="AP38" s="40"/>
+      <c r="AQ38" s="40"/>
+      <c r="AR38" s="40"/>
+    </row>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
       <c r="B39" s="41" t="s">
         <v>135</v>
       </c>
@@ -8896,7 +9798,7 @@
       <c r="N39" s="42">
         <v>0.12786700000000001</v>
       </c>
-      <c r="P39" s="63"/>
+      <c r="P39" s="60"/>
       <c r="Q39" s="41" t="s">
         <v>135</v>
       </c>
@@ -8930,8 +9832,24 @@
       <c r="AC39" s="42">
         <v>0.94489999999999996</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE39" s="60"/>
+      <c r="AF39" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG39" s="41"/>
+      <c r="AH39" s="41"/>
+      <c r="AI39" s="41"/>
+      <c r="AJ39" s="41"/>
+      <c r="AK39" s="41"/>
+      <c r="AL39" s="41"/>
+      <c r="AM39" s="41"/>
+      <c r="AN39" s="41"/>
+      <c r="AO39" s="41"/>
+      <c r="AP39" s="42"/>
+      <c r="AQ39" s="42"/>
+      <c r="AR39" s="42"/>
+    </row>
+    <row r="40" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="L40" s="32"/>
       <c r="M40" s="32"/>
@@ -8941,7 +9859,7 @@
       <c r="AB40" s="32"/>
       <c r="AC40" s="32"/>
     </row>
-    <row r="41" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
@@ -8951,7 +9869,7 @@
       <c r="AB41" s="32"/>
       <c r="AC41" s="32"/>
     </row>
-    <row r="42" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="L42" s="32"/>
       <c r="M42" s="32"/>
@@ -8961,7 +9879,7 @@
       <c r="AB42" s="32"/>
       <c r="AC42" s="32"/>
     </row>
-    <row r="43" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="L43" s="32"/>
       <c r="M43" s="32"/>
@@ -8971,7 +9889,7 @@
       <c r="AB43" s="32"/>
       <c r="AC43" s="32"/>
     </row>
-    <row r="44" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="L44" s="32"/>
       <c r="M44" s="32"/>
@@ -8981,7 +9899,7 @@
       <c r="AB44" s="32"/>
       <c r="AC44" s="32"/>
     </row>
-    <row r="45" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="L45" s="32"/>
       <c r="M45" s="32"/>
@@ -8991,7 +9909,7 @@
       <c r="AB45" s="32"/>
       <c r="AC45" s="32"/>
     </row>
-    <row r="46" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
@@ -9001,7 +9919,7 @@
       <c r="AB46" s="32"/>
       <c r="AC46" s="32"/>
     </row>
-    <row r="47" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="L47" s="32"/>
       <c r="M47" s="32"/>
@@ -9011,7 +9929,7 @@
       <c r="AB47" s="32"/>
       <c r="AC47" s="32"/>
     </row>
-    <row r="48" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="L48" s="32"/>
       <c r="M48" s="32"/>
@@ -11032,7 +11950,7 @@
       <c r="AC249" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="48">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="P1:AC1"/>
     <mergeCell ref="L2:N2"/>
@@ -11065,6 +11983,22 @@
     <mergeCell ref="P28:P31"/>
     <mergeCell ref="P32:P35"/>
     <mergeCell ref="P36:P39"/>
+    <mergeCell ref="AE1:AR1"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AE24:AE27"/>
+    <mergeCell ref="AE28:AE31"/>
+    <mergeCell ref="AE32:AE35"/>
+    <mergeCell ref="AE36:AE39"/>
+    <mergeCell ref="AE4:AE7"/>
+    <mergeCell ref="AE8:AE11"/>
+    <mergeCell ref="AE12:AE15"/>
+    <mergeCell ref="AE16:AE19"/>
+    <mergeCell ref="AE20:AE23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -11095,27 +12029,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="66" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="66" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="69" t="s">
         <v>128</v>
       </c>
@@ -11123,8 +12057,8 @@
       <c r="N1" s="71"/>
     </row>
     <row r="2" spans="1:17" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="36" t="s">
         <v>125</v>
       </c>
@@ -11164,7 +12098,7 @@
       <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="57" t="s">
         <v>136</v>
       </c>
       <c r="B3" s="38" t="s">
@@ -11205,7 +12139,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="38" t="s">
         <v>133</v>
       </c>
@@ -11247,7 +12181,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="38" t="s">
         <v>134</v>
       </c>
@@ -11283,7 +12217,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="41" t="s">
         <v>135</v>
       </c>
@@ -11316,7 +12250,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="57" t="s">
         <v>137</v>
       </c>
       <c r="B7" s="38" t="s">
@@ -11354,7 +12288,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="38" t="s">
         <v>133</v>
       </c>
@@ -11396,7 +12330,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="38" t="s">
         <v>134</v>
       </c>
@@ -11432,7 +12366,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="41" t="s">
         <v>135</v>
       </c>
@@ -11462,7 +12396,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="38" t="s">
@@ -11500,7 +12434,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="38" t="s">
         <v>133</v>
       </c>
@@ -11536,7 +12470,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="38" t="s">
         <v>134</v>
       </c>
@@ -11572,7 +12506,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="41" t="s">
         <v>135</v>
       </c>
@@ -11602,7 +12536,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="61" t="s">
         <v>138</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -11644,7 +12578,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="39" t="s">
         <v>133</v>
       </c>
@@ -11683,7 +12617,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="38" t="s">
         <v>134</v>
       </c>
@@ -11719,7 +12653,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
+      <c r="A18" s="63"/>
       <c r="B18" s="41" t="s">
         <v>135</v>
       </c>
@@ -11751,7 +12685,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="61" t="s">
         <v>139</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -11789,7 +12723,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="38" t="s">
         <v>133</v>
       </c>
@@ -11825,7 +12759,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="38" t="s">
         <v>134</v>
       </c>
@@ -11861,7 +12795,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="41" t="s">
         <v>135</v>
       </c>
@@ -11893,7 +12827,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="57" t="s">
         <v>140</v>
       </c>
       <c r="B23" s="38" t="s">
@@ -11931,7 +12865,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="38" t="s">
         <v>133</v>
       </c>
@@ -11967,7 +12901,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="38" t="s">
         <v>134</v>
       </c>
@@ -12005,7 +12939,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="41" t="s">
         <v>135</v>
       </c>
@@ -12035,7 +12969,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="57" t="s">
         <v>116</v>
       </c>
       <c r="B27" s="38" t="s">
@@ -12073,7 +13007,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="38" t="s">
         <v>133</v>
       </c>
@@ -12109,7 +13043,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="38" t="s">
         <v>134</v>
       </c>
@@ -12145,7 +13079,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="41" t="s">
         <v>135</v>
       </c>
@@ -12175,7 +13109,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="57" t="s">
         <v>141</v>
       </c>
       <c r="B31" s="38" t="s">
@@ -12213,7 +13147,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="38" t="s">
         <v>133</v>
       </c>
@@ -12249,7 +13183,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="38" t="s">
         <v>134</v>
       </c>
@@ -12287,7 +13221,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="41" t="s">
         <v>135</v>
       </c>
@@ -12321,7 +13255,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="60" t="s">
         <v>142</v>
       </c>
       <c r="B35" s="38" t="s">
@@ -12359,7 +13293,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="63"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="38" t="s">
         <v>133</v>
       </c>
@@ -12395,7 +13329,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="63"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="38" t="s">
         <v>134</v>
       </c>
@@ -12437,7 +13371,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="63"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="41" t="s">
         <v>135</v>
       </c>
@@ -18701,13 +19635,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change for sinchronization analysis
</commit_message>
<xml_diff>
--- a/DataSet_VersionRecuperada.xlsx
+++ b/DataSet_VersionRecuperada.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Group 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Totales" sheetId="5" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="10" r:id="rId8"/>
     <sheet name="Hoja2" sheetId="11" r:id="rId9"/>
+    <sheet name="Sincronization" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group 1'!$A$1:$AV$19</definedName>
@@ -116,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="181">
   <si>
     <t>7:00 a 8:00</t>
   </si>
@@ -944,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1111,6 +1112,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1192,11 +1199,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1647,7 +1660,7 @@
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1779,7 +1792,7 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1920,7 +1933,7 @@
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="56"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2064,7 +2077,7 @@
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="56"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2348,7 +2361,7 @@
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="56"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2492,7 +2505,7 @@
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2646,7 @@
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="56"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2777,7 +2790,7 @@
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2918,7 +2931,7 @@
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="58">
         <v>43555</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -3061,7 +3074,7 @@
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3205,7 +3218,7 @@
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="58">
         <v>43561</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -3348,7 +3361,7 @@
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
@@ -3492,7 +3505,7 @@
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -3636,7 +3649,7 @@
       <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
@@ -3774,7 +3787,7 @@
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3915,7 +3928,7 @@
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4056,7 +4069,7 @@
       <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="56"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
@@ -5030,6 +5043,1108 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="68"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="86">
+        <v>1</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="86"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="88">
+        <v>3.5309399999999998E-2</v>
+      </c>
+      <c r="M4" s="88">
+        <v>0.17068800000000001</v>
+      </c>
+      <c r="N4" s="88">
+        <v>0.21309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="60"/>
+      <c r="B5" s="86">
+        <v>2</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="86"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="87"/>
+      <c r="L5" s="88">
+        <v>8.57768E-2</v>
+      </c>
+      <c r="M5" s="88">
+        <v>6.2725100000000006E-2</v>
+      </c>
+      <c r="N5" s="88">
+        <v>4.8309499999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="86">
+        <v>3</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88">
+        <v>0.16553100000000001</v>
+      </c>
+      <c r="M6" s="88">
+        <v>2.7691400000000001E-2</v>
+      </c>
+      <c r="N6" s="88">
+        <v>3.1797300000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="86">
+        <v>4</v>
+      </c>
+      <c r="C7" s="86"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="87"/>
+      <c r="L7" s="88">
+        <v>0.113597</v>
+      </c>
+      <c r="M7" s="88">
+        <v>0.20688300000000001</v>
+      </c>
+      <c r="N7" s="88">
+        <v>0.21010699999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="86">
+        <v>5</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="87"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" s="87"/>
+      <c r="L8" s="88">
+        <v>1.91167E-2</v>
+      </c>
+      <c r="M8" s="88">
+        <v>5.7552800000000001E-2</v>
+      </c>
+      <c r="N8" s="88">
+        <v>0.19677700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="86">
+        <v>1</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="87"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="88">
+        <v>4.3114899999999998E-2</v>
+      </c>
+      <c r="M9" s="88">
+        <v>6.0272600000000003E-2</v>
+      </c>
+      <c r="N9" s="88">
+        <v>4.5336700000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="86">
+        <v>2</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="88">
+        <v>0.10954899999999999</v>
+      </c>
+      <c r="M10" s="88">
+        <v>1.7465700000000001E-2</v>
+      </c>
+      <c r="N10" s="88">
+        <v>1.7925099999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="60"/>
+      <c r="B11" s="86">
+        <v>3</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88">
+        <v>0.122132</v>
+      </c>
+      <c r="M11" s="88">
+        <v>0.175541</v>
+      </c>
+      <c r="N11" s="88">
+        <v>4.7662099999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+      <c r="B12" s="86">
+        <v>4</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="87"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="87"/>
+      <c r="L12" s="88">
+        <v>6.7224999999999993E-2</v>
+      </c>
+      <c r="M12" s="88">
+        <v>8.6080299999999998E-2</v>
+      </c>
+      <c r="N12" s="88">
+        <v>0.119604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="61"/>
+      <c r="B13" s="86">
+        <v>5</v>
+      </c>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="88">
+        <v>0.208122</v>
+      </c>
+      <c r="M13" s="88">
+        <v>0.146788</v>
+      </c>
+      <c r="N13" s="88">
+        <v>0.22092400000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="86">
+        <v>1</v>
+      </c>
+      <c r="C14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="86">
+        <v>2</v>
+      </c>
+      <c r="C15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="60"/>
+      <c r="B16" s="86">
+        <v>3</v>
+      </c>
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="88"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="60"/>
+      <c r="B17" s="86">
+        <v>4</v>
+      </c>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="88"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="61"/>
+      <c r="B18" s="86">
+        <v>5</v>
+      </c>
+      <c r="C18" s="86"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="86">
+        <v>1</v>
+      </c>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="64"/>
+      <c r="B20" s="86">
+        <v>2</v>
+      </c>
+      <c r="C20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="64"/>
+      <c r="B21" s="86">
+        <v>3</v>
+      </c>
+      <c r="C21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="64"/>
+      <c r="B22" s="86">
+        <v>4</v>
+      </c>
+      <c r="C22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="65"/>
+      <c r="B23" s="86">
+        <v>5</v>
+      </c>
+      <c r="C23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="86">
+        <v>1</v>
+      </c>
+      <c r="C24" s="86"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="87"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="64"/>
+      <c r="B25" s="86">
+        <v>2</v>
+      </c>
+      <c r="C25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="87"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="64"/>
+      <c r="B26" s="86">
+        <v>3</v>
+      </c>
+      <c r="C26" s="86"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88"/>
+      <c r="N26" s="88"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="64"/>
+      <c r="B27" s="86">
+        <v>4</v>
+      </c>
+      <c r="C27" s="86"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="65"/>
+      <c r="B28" s="86">
+        <v>5</v>
+      </c>
+      <c r="C28" s="86"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="88"/>
+      <c r="M28" s="88"/>
+      <c r="N28" s="88"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="86">
+        <v>1</v>
+      </c>
+      <c r="C29" s="86"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="88"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="86">
+        <v>2</v>
+      </c>
+      <c r="C30" s="86"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="86">
+        <v>3</v>
+      </c>
+      <c r="C31" s="86"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="86">
+        <v>4</v>
+      </c>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="61"/>
+      <c r="B33" s="86">
+        <v>5</v>
+      </c>
+      <c r="C33" s="86"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="87"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="86">
+        <v>1</v>
+      </c>
+      <c r="C34" s="86"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="88"/>
+      <c r="M34" s="88"/>
+      <c r="N34" s="88"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="86">
+        <v>2</v>
+      </c>
+      <c r="C35" s="86"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="87"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
+      <c r="N35" s="88"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="60"/>
+      <c r="B36" s="86">
+        <v>3</v>
+      </c>
+      <c r="C36" s="86"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="87"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="87"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="88"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="60"/>
+      <c r="B37" s="86">
+        <v>4</v>
+      </c>
+      <c r="C37" s="86"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="87"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="87"/>
+      <c r="K37" s="87"/>
+      <c r="L37" s="88"/>
+      <c r="M37" s="88"/>
+      <c r="N37" s="88"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="61"/>
+      <c r="B38" s="86">
+        <v>5</v>
+      </c>
+      <c r="C38" s="86"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
+      <c r="N38" s="88"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="86">
+        <v>1</v>
+      </c>
+      <c r="C39" s="86"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="87"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="87"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="88"/>
+      <c r="M39" s="88"/>
+      <c r="N39" s="88"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="60"/>
+      <c r="B40" s="86">
+        <v>2</v>
+      </c>
+      <c r="C40" s="86"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="88"/>
+      <c r="M40" s="88"/>
+      <c r="N40" s="88"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="60"/>
+      <c r="B41" s="86">
+        <v>3</v>
+      </c>
+      <c r="C41" s="86"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="86"/>
+      <c r="J41" s="87"/>
+      <c r="K41" s="87"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="88"/>
+      <c r="N41" s="88"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="60"/>
+      <c r="B42" s="86">
+        <v>4</v>
+      </c>
+      <c r="C42" s="86"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="88"/>
+      <c r="M42" s="88"/>
+      <c r="N42" s="88"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="61"/>
+      <c r="B43" s="86">
+        <v>5</v>
+      </c>
+      <c r="C43" s="86"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="86"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="88"/>
+      <c r="N43" s="88"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="86">
+        <v>1</v>
+      </c>
+      <c r="C44" s="86"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="88"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="62"/>
+      <c r="B45" s="86">
+        <v>2</v>
+      </c>
+      <c r="C45" s="86"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="62"/>
+      <c r="B46" s="86">
+        <v>3</v>
+      </c>
+      <c r="C46" s="86"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="87"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="87"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
+      <c r="N46" s="88"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="62"/>
+      <c r="B47" s="86">
+        <v>4</v>
+      </c>
+      <c r="C47" s="86"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="87"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="88"/>
+      <c r="N47" s="88"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="62"/>
+      <c r="B48" s="86">
+        <v>5</v>
+      </c>
+      <c r="C48" s="86"/>
+      <c r="D48" s="87"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="87"/>
+      <c r="I48" s="86"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="88"/>
+      <c r="M48" s="88"/>
+      <c r="N48" s="88"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="85"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="85"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="85"/>
+      <c r="I49" s="85"/>
+      <c r="J49" s="85"/>
+      <c r="K49" s="85"/>
+      <c r="L49" s="85"/>
+      <c r="M49" s="85"/>
+      <c r="N49" s="85"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="85"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="85"/>
+      <c r="K50" s="85"/>
+      <c r="L50" s="85"/>
+      <c r="M50" s="85"/>
+      <c r="N50" s="85"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5205,7 +6320,7 @@
       <c r="A2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="58">
         <v>43548</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5289,7 +6404,7 @@
       <c r="A3" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -5371,7 +6486,7 @@
       <c r="A4" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="56"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
@@ -5453,7 +6568,7 @@
       <c r="A5" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="56"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -5535,7 +6650,7 @@
       <c r="A6" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -5617,7 +6732,7 @@
       <c r="A7" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="56"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -5699,7 +6814,7 @@
       <c r="A8" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
@@ -5778,7 +6893,7 @@
       <c r="A9" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="56"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="44">
         <v>0.25</v>
       </c>
@@ -6271,8 +7386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AC39"/>
+    <sheetView topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AR39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6311,138 +7426,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="66"/>
-      <c r="P1" s="64" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="68"/>
+      <c r="P1" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="66"/>
-      <c r="AE1" s="64" t="s">
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="68"/>
+      <c r="AE1" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="65"/>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="66"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="68"/>
     </row>
     <row r="2" spans="1:44" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="64" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="64" t="s">
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="69" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
-      <c r="P2" s="67" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+      <c r="P2" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="67" t="s">
+      <c r="Q2" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="R2" s="64" t="s">
+      <c r="R2" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="S2" s="65"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="64" t="s">
+      <c r="S2" s="67"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="64" t="s">
+      <c r="V2" s="67"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="69" t="s">
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="71"/>
-      <c r="AE2" s="67" t="s">
+      <c r="AB2" s="72"/>
+      <c r="AC2" s="73"/>
+      <c r="AE2" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="AF2" s="67" t="s">
+      <c r="AF2" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="AG2" s="64" t="s">
+      <c r="AG2" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="64" t="s">
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="68"/>
+      <c r="AJ2" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="AK2" s="65"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="64" t="s">
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="68"/>
+      <c r="AM2" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="69" t="s">
+      <c r="AN2" s="67"/>
+      <c r="AO2" s="68"/>
+      <c r="AP2" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="AQ2" s="70"/>
-      <c r="AR2" s="71"/>
+      <c r="AQ2" s="72"/>
+      <c r="AR2" s="73"/>
     </row>
     <row r="3" spans="1:44" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="36" t="s">
         <v>125</v>
       </c>
@@ -6479,8 +7594,8 @@
       <c r="N3" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
       <c r="R3" s="36" t="s">
         <v>125</v>
       </c>
@@ -6517,8 +7632,8 @@
       <c r="AC3" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
+      <c r="AE3" s="70"/>
+      <c r="AF3" s="70"/>
       <c r="AG3" s="36" t="s">
         <v>125</v>
       </c>
@@ -6557,7 +7672,7 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="59" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="38" t="s">
@@ -6596,7 +7711,7 @@
       <c r="O4" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="P4" s="57" t="s">
+      <c r="P4" s="59" t="s">
         <v>136</v>
       </c>
       <c r="Q4" s="38" t="s">
@@ -6632,27 +7747,45 @@
       <c r="AC4" s="40">
         <v>0.80864800000000003</v>
       </c>
-      <c r="AE4" s="57" t="s">
+      <c r="AE4" s="59" t="s">
         <v>136</v>
       </c>
       <c r="AF4" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="39"/>
-      <c r="AL4" s="38"/>
+      <c r="AG4" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH4" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI4" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ4" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK4" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL4" s="38" t="s">
+        <v>108</v>
+      </c>
       <c r="AM4" s="38"/>
       <c r="AN4" s="39"/>
       <c r="AO4" s="38"/>
-      <c r="AP4" s="40"/>
-      <c r="AQ4" s="40"/>
-      <c r="AR4" s="40"/>
+      <c r="AP4" s="40">
+        <v>0.72185900000000003</v>
+      </c>
+      <c r="AQ4" s="40">
+        <v>0.14366699999999999</v>
+      </c>
+      <c r="AR4" s="40">
+        <v>6.3313099999999997E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="38" t="s">
         <v>133</v>
       </c>
@@ -6674,13 +7807,13 @@
       <c r="H5" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" s="84" t="s">
+      <c r="I5" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="57" t="s">
         <v>108</v>
       </c>
       <c r="L5" s="40">
@@ -6692,7 +7825,7 @@
       <c r="N5" s="40">
         <v>0.53922099999999995</v>
       </c>
-      <c r="P5" s="58"/>
+      <c r="P5" s="60"/>
       <c r="Q5" s="38" t="s">
         <v>133</v>
       </c>
@@ -6714,13 +7847,13 @@
       <c r="W5" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X5" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y5" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z5" s="84" t="s">
+      <c r="X5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y5" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AA5" s="40">
@@ -6732,25 +7865,49 @@
       <c r="AC5" s="40">
         <v>0.74212500000000003</v>
       </c>
-      <c r="AE5" s="58"/>
+      <c r="AE5" s="60"/>
       <c r="AF5" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="39"/>
-      <c r="AI5" s="39"/>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="39"/>
-      <c r="AL5" s="39"/>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="39"/>
-      <c r="AO5" s="39"/>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
+      <c r="AG5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH5" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI5" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK5" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL5" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM5" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN5" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO5" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP5" s="40">
+        <v>7.6537400000000005E-2</v>
+      </c>
+      <c r="AQ5" s="40">
+        <v>2.2092799999999999E-2</v>
+      </c>
+      <c r="AR5" s="40">
+        <v>0.48709999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="38" t="s">
         <v>134</v>
       </c>
@@ -6786,7 +7943,7 @@
       <c r="N6" s="40">
         <v>4.9845799999999997E-3</v>
       </c>
-      <c r="P6" s="58"/>
+      <c r="P6" s="60"/>
       <c r="Q6" s="38" t="s">
         <v>134</v>
       </c>
@@ -6820,25 +7977,47 @@
       <c r="AC6" s="40">
         <v>0.32851900000000001</v>
       </c>
-      <c r="AE6" s="58"/>
+      <c r="AE6" s="60"/>
       <c r="AF6" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="39"/>
-      <c r="AI6" s="39"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="39"/>
-      <c r="AL6" s="39"/>
+      <c r="AG6" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH6" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ6" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK6" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL6" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM6" s="38"/>
-      <c r="AN6" s="39"/>
-      <c r="AO6" s="39"/>
-      <c r="AP6" s="40"/>
-      <c r="AQ6" s="40"/>
-      <c r="AR6" s="40"/>
+      <c r="AN6" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO6" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP6" s="40">
+        <v>3.8796799999999999E-2</v>
+      </c>
+      <c r="AQ6" s="40">
+        <v>2.2092799999999999E-2</v>
+      </c>
+      <c r="AR6" s="40">
+        <v>2.13978E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="41" t="s">
         <v>135</v>
       </c>
@@ -6860,7 +8039,7 @@
       <c r="N7" s="42">
         <v>6.9331199999999996E-4</v>
       </c>
-      <c r="P7" s="59"/>
+      <c r="P7" s="61"/>
       <c r="Q7" s="41" t="s">
         <v>135</v>
       </c>
@@ -6882,25 +8061,31 @@
       <c r="AC7" s="42">
         <v>5.0963000000000001E-2</v>
       </c>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="41" t="s">
+      <c r="AE7" s="61"/>
+      <c r="AF7" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG7" s="41"/>
-      <c r="AH7" s="41"/>
-      <c r="AI7" s="41"/>
-      <c r="AJ7" s="41"/>
-      <c r="AK7" s="41"/>
-      <c r="AL7" s="41"/>
-      <c r="AM7" s="41"/>
-      <c r="AN7" s="41"/>
-      <c r="AO7" s="41"/>
-      <c r="AP7" s="42"/>
-      <c r="AQ7" s="42"/>
-      <c r="AR7" s="42"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="39"/>
+      <c r="AI7" s="39"/>
+      <c r="AJ7" s="38"/>
+      <c r="AK7" s="39"/>
+      <c r="AL7" s="39"/>
+      <c r="AM7" s="38"/>
+      <c r="AN7" s="39"/>
+      <c r="AO7" s="39"/>
+      <c r="AP7" s="40">
+        <v>4.0784200000000001E-3</v>
+      </c>
+      <c r="AQ7" s="40">
+        <v>2.7042799999999999E-3</v>
+      </c>
+      <c r="AR7" s="40">
+        <v>5.1244800000000001E-5</v>
+      </c>
     </row>
     <row r="8" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="59" t="s">
         <v>137</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -6936,7 +8121,7 @@
       <c r="N8" s="40">
         <v>0.34474100000000002</v>
       </c>
-      <c r="P8" s="57" t="s">
+      <c r="P8" s="59" t="s">
         <v>137</v>
       </c>
       <c r="Q8" s="38" t="s">
@@ -6972,27 +8157,45 @@
       <c r="AC8" s="40">
         <v>0.83276700000000003</v>
       </c>
-      <c r="AE8" s="57" t="s">
+      <c r="AE8" s="59" t="s">
         <v>137</v>
       </c>
       <c r="AF8" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
-      <c r="AI8" s="39"/>
-      <c r="AJ8" s="38"/>
-      <c r="AK8" s="38"/>
-      <c r="AL8" s="39"/>
+      <c r="AG8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI8" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL8" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM8" s="38"/>
       <c r="AN8" s="38"/>
       <c r="AO8" s="38"/>
-      <c r="AP8" s="40"/>
-      <c r="AQ8" s="40"/>
-      <c r="AR8" s="40"/>
+      <c r="AP8" s="40">
+        <v>0.86891399999999996</v>
+      </c>
+      <c r="AQ8" s="40">
+        <v>0.62708399999999997</v>
+      </c>
+      <c r="AR8" s="40">
+        <v>0.35993000000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="38" t="s">
         <v>133</v>
       </c>
@@ -7014,13 +8217,13 @@
       <c r="H9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="J9" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="84" t="s">
+      <c r="I9" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="57" t="s">
         <v>108</v>
       </c>
       <c r="L9" s="40">
@@ -7032,7 +8235,7 @@
       <c r="N9" s="40">
         <v>0.93847400000000003</v>
       </c>
-      <c r="P9" s="58"/>
+      <c r="P9" s="60"/>
       <c r="Q9" s="38" t="s">
         <v>133</v>
       </c>
@@ -7054,13 +8257,13 @@
       <c r="W9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X9" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y9" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z9" s="84" t="s">
+      <c r="X9" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y9" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z9" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AA9" s="40">
@@ -7072,25 +8275,49 @@
       <c r="AC9" s="40">
         <v>0.36027500000000001</v>
       </c>
-      <c r="AE9" s="58"/>
+      <c r="AE9" s="60"/>
       <c r="AF9" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="39"/>
-      <c r="AJ9" s="38"/>
-      <c r="AK9" s="38"/>
-      <c r="AL9" s="39"/>
-      <c r="AM9" s="38"/>
-      <c r="AN9" s="38"/>
-      <c r="AO9" s="39"/>
-      <c r="AP9" s="40"/>
-      <c r="AQ9" s="40"/>
-      <c r="AR9" s="40"/>
+      <c r="AG9" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH9" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI9" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ9" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK9" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL9" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM9" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN9" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO9" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP9" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="AQ9" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="AR9" s="40">
+        <v>0.63156500000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="38" t="s">
         <v>134</v>
       </c>
@@ -7126,7 +8353,7 @@
       <c r="N10" s="40">
         <v>1.1750500000000001E-2</v>
       </c>
-      <c r="P10" s="58"/>
+      <c r="P10" s="60"/>
       <c r="Q10" s="38" t="s">
         <v>134</v>
       </c>
@@ -7160,25 +8387,49 @@
       <c r="AC10" s="40">
         <v>0.42157099999999997</v>
       </c>
-      <c r="AE10" s="58"/>
+      <c r="AE10" s="60"/>
       <c r="AF10" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="39"/>
-      <c r="AJ10" s="38"/>
-      <c r="AK10" s="38"/>
-      <c r="AL10" s="39"/>
-      <c r="AM10" s="38"/>
-      <c r="AN10" s="38"/>
-      <c r="AO10" s="39"/>
-      <c r="AP10" s="40"/>
-      <c r="AQ10" s="40"/>
-      <c r="AR10" s="40"/>
+      <c r="AG10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI10" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL10" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN10" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO10" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP10" s="40">
+        <v>1.8550500000000001E-2</v>
+      </c>
+      <c r="AQ10" s="40">
+        <v>2.2803400000000001E-2</v>
+      </c>
+      <c r="AR10" s="40">
+        <v>5.0504499999999997E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:44" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="41" t="s">
         <v>135</v>
       </c>
@@ -7200,7 +8451,7 @@
       <c r="N11" s="42">
         <v>4.1270400000000002E-3</v>
       </c>
-      <c r="P11" s="59"/>
+      <c r="P11" s="61"/>
       <c r="Q11" s="41" t="s">
         <v>135</v>
       </c>
@@ -7228,25 +8479,35 @@
       <c r="AC11" s="42">
         <v>8.3578299999999994E-2</v>
       </c>
-      <c r="AE11" s="59"/>
-      <c r="AF11" s="41" t="s">
+      <c r="AE11" s="61"/>
+      <c r="AF11" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG11" s="41"/>
-      <c r="AH11" s="41"/>
-      <c r="AI11" s="41"/>
-      <c r="AJ11" s="41"/>
-      <c r="AK11" s="41"/>
-      <c r="AL11" s="41"/>
-      <c r="AM11" s="41"/>
-      <c r="AN11" s="41"/>
-      <c r="AO11" s="41"/>
-      <c r="AP11" s="42"/>
-      <c r="AQ11" s="42"/>
-      <c r="AR11" s="42"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="39"/>
+      <c r="AI11" s="39"/>
+      <c r="AJ11" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK11" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL11" s="39"/>
+      <c r="AM11" s="38"/>
+      <c r="AN11" s="39"/>
+      <c r="AO11" s="39"/>
+      <c r="AP11" s="40">
+        <v>1.5259699999999999E-2</v>
+      </c>
+      <c r="AQ11" s="40">
+        <v>9.72809E-3</v>
+      </c>
+      <c r="AR11" s="40">
+        <v>2.9956699999999999E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="59" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="38" t="s">
@@ -7282,7 +8543,7 @@
       <c r="N12" s="40">
         <v>0.61764799999999997</v>
       </c>
-      <c r="P12" s="57" t="s">
+      <c r="P12" s="59" t="s">
         <v>110</v>
       </c>
       <c r="Q12" s="38" t="s">
@@ -7318,27 +8579,45 @@
       <c r="AC12" s="40">
         <v>0.72725300000000004</v>
       </c>
-      <c r="AE12" s="57" t="s">
+      <c r="AE12" s="59" t="s">
         <v>110</v>
       </c>
       <c r="AF12" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG12" s="38"/>
-      <c r="AH12" s="39"/>
-      <c r="AI12" s="38"/>
-      <c r="AJ12" s="38"/>
-      <c r="AK12" s="39"/>
-      <c r="AL12" s="38"/>
+      <c r="AG12" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH12" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI12" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ12" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK12" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL12" s="38" t="s">
+        <v>108</v>
+      </c>
       <c r="AM12" s="38"/>
       <c r="AN12" s="39"/>
       <c r="AO12" s="38"/>
-      <c r="AP12" s="40"/>
-      <c r="AQ12" s="40"/>
-      <c r="AR12" s="40"/>
+      <c r="AP12" s="40">
+        <v>0.155637</v>
+      </c>
+      <c r="AQ12" s="40">
+        <v>0.183336</v>
+      </c>
+      <c r="AR12" s="40">
+        <v>0.29955799999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="38" t="s">
         <v>133</v>
       </c>
@@ -7372,7 +8651,7 @@
       <c r="N13" s="40">
         <v>0.18202299999999999</v>
       </c>
-      <c r="P13" s="58"/>
+      <c r="P13" s="60"/>
       <c r="Q13" s="38" t="s">
         <v>133</v>
       </c>
@@ -7406,25 +8685,43 @@
       <c r="AC13" s="40">
         <v>0.50264500000000001</v>
       </c>
-      <c r="AE13" s="58"/>
+      <c r="AE13" s="60"/>
       <c r="AF13" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG13" s="38"/>
-      <c r="AH13" s="39"/>
-      <c r="AI13" s="39"/>
-      <c r="AJ13" s="38"/>
-      <c r="AK13" s="39"/>
-      <c r="AL13" s="39"/>
+      <c r="AG13" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH13" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI13" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ13" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK13" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL13" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM13" s="38"/>
       <c r="AN13" s="39"/>
       <c r="AO13" s="39"/>
-      <c r="AP13" s="40"/>
-      <c r="AQ13" s="40"/>
-      <c r="AR13" s="40"/>
+      <c r="AP13" s="40">
+        <v>1.28065E-2</v>
+      </c>
+      <c r="AQ13" s="40">
+        <v>1.8652100000000001E-2</v>
+      </c>
+      <c r="AR13" s="40">
+        <v>4.23083E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="38" t="s">
         <v>134</v>
       </c>
@@ -7458,7 +8755,7 @@
       <c r="N14" s="40">
         <v>5.4985399999999997E-2</v>
       </c>
-      <c r="P14" s="58"/>
+      <c r="P14" s="60"/>
       <c r="Q14" s="38" t="s">
         <v>134</v>
       </c>
@@ -7492,25 +8789,43 @@
       <c r="AC14" s="40">
         <v>0.35624899999999998</v>
       </c>
-      <c r="AE14" s="58"/>
+      <c r="AE14" s="60"/>
       <c r="AF14" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="39"/>
-      <c r="AI14" s="39"/>
-      <c r="AJ14" s="38"/>
-      <c r="AK14" s="39"/>
-      <c r="AL14" s="39"/>
+      <c r="AG14" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH14" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI14" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ14" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK14" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL14" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM14" s="38"/>
       <c r="AN14" s="39"/>
       <c r="AO14" s="39"/>
-      <c r="AP14" s="40"/>
-      <c r="AQ14" s="40"/>
-      <c r="AR14" s="40"/>
+      <c r="AP14" s="40">
+        <v>0.22331999999999999</v>
+      </c>
+      <c r="AQ14" s="40">
+        <v>2.27297E-3</v>
+      </c>
+      <c r="AR14" s="40">
+        <v>1.6263400000000001E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="41" t="s">
         <v>135</v>
       </c>
@@ -7532,7 +8847,7 @@
       <c r="N15" s="42">
         <v>0</v>
       </c>
-      <c r="P15" s="59"/>
+      <c r="P15" s="61"/>
       <c r="Q15" s="41" t="s">
         <v>135</v>
       </c>
@@ -7560,25 +8875,33 @@
       <c r="AC15" s="42">
         <v>0.228573</v>
       </c>
-      <c r="AE15" s="59"/>
-      <c r="AF15" s="41" t="s">
+      <c r="AE15" s="61"/>
+      <c r="AF15" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG15" s="41"/>
-      <c r="AH15" s="41"/>
-      <c r="AI15" s="41"/>
-      <c r="AJ15" s="41"/>
-      <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="41"/>
-      <c r="AN15" s="41"/>
-      <c r="AO15" s="41"/>
-      <c r="AP15" s="42"/>
-      <c r="AQ15" s="42"/>
-      <c r="AR15" s="42"/>
+      <c r="AG15" s="38"/>
+      <c r="AH15" s="39"/>
+      <c r="AI15" s="39"/>
+      <c r="AJ15" s="38"/>
+      <c r="AK15" s="39"/>
+      <c r="AL15" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM15" s="38"/>
+      <c r="AN15" s="39"/>
+      <c r="AO15" s="39"/>
+      <c r="AP15" s="40">
+        <v>0.244815</v>
+      </c>
+      <c r="AQ15" s="40">
+        <v>3.7187800000000003E-5</v>
+      </c>
+      <c r="AR15" s="40">
+        <v>1.84249E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="63" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="39" t="s">
@@ -7602,7 +8925,7 @@
       <c r="H16" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="83" t="s">
+      <c r="I16" s="56" t="s">
         <v>108</v>
       </c>
       <c r="J16" s="39"/>
@@ -7616,7 +8939,7 @@
       <c r="N16" s="40">
         <v>0.29320299999999999</v>
       </c>
-      <c r="P16" s="61" t="s">
+      <c r="P16" s="63" t="s">
         <v>138</v>
       </c>
       <c r="Q16" s="39" t="s">
@@ -7640,7 +8963,7 @@
       <c r="W16" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X16" s="83" t="s">
+      <c r="X16" s="56" t="s">
         <v>108</v>
       </c>
       <c r="Y16" s="39" t="s">
@@ -7656,7 +8979,7 @@
       <c r="AC16" s="40">
         <v>0.81892100000000001</v>
       </c>
-      <c r="AE16" s="61" t="s">
+      <c r="AE16" s="63" t="s">
         <v>138</v>
       </c>
       <c r="AF16" s="39" t="s">
@@ -7680,10 +9003,10 @@
       <c r="AL16" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="AM16" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="AN16" s="39" t="s">
+      <c r="AM16" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN16" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AO16" s="39" t="s">
@@ -7700,7 +9023,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="39" t="s">
         <v>133</v>
       </c>
@@ -7734,7 +9057,7 @@
       <c r="N17" s="40">
         <v>0.174321</v>
       </c>
-      <c r="P17" s="62"/>
+      <c r="P17" s="64"/>
       <c r="Q17" s="39" t="s">
         <v>133</v>
       </c>
@@ -7768,7 +9091,7 @@
       <c r="AC17" s="40">
         <v>0.46240999999999999</v>
       </c>
-      <c r="AE17" s="62"/>
+      <c r="AE17" s="64"/>
       <c r="AF17" s="39" t="s">
         <v>133</v>
       </c>
@@ -7791,10 +9114,10 @@
         <v>108</v>
       </c>
       <c r="AM17" s="38"/>
-      <c r="AN17" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="AO17" s="39" t="s">
+      <c r="AN17" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO17" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AP17" s="40">
@@ -7808,7 +9131,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="38" t="s">
         <v>134</v>
       </c>
@@ -7846,7 +9169,7 @@
       <c r="N18" s="40">
         <v>1.3136500000000001E-2</v>
       </c>
-      <c r="P18" s="62"/>
+      <c r="P18" s="64"/>
       <c r="Q18" s="38" t="s">
         <v>134</v>
       </c>
@@ -7880,7 +9203,7 @@
       <c r="AC18" s="40">
         <v>0.97048199999999996</v>
       </c>
-      <c r="AE18" s="62"/>
+      <c r="AE18" s="64"/>
       <c r="AF18" s="38" t="s">
         <v>134</v>
       </c>
@@ -7902,13 +9225,13 @@
       <c r="AL18" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="AM18" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="AN18" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="AO18" s="39" t="s">
+      <c r="AM18" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN18" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO18" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AP18" s="40">
@@ -7922,7 +9245,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="41" t="s">
         <v>135</v>
       </c>
@@ -7944,7 +9267,7 @@
       <c r="N19" s="42">
         <v>3.6087900000000002E-3</v>
       </c>
-      <c r="P19" s="63"/>
+      <c r="P19" s="65"/>
       <c r="Q19" s="41" t="s">
         <v>135</v>
       </c>
@@ -7974,35 +9297,35 @@
       <c r="AC19" s="42">
         <v>0.75703299999999996</v>
       </c>
-      <c r="AE19" s="63"/>
-      <c r="AF19" s="41" t="s">
+      <c r="AE19" s="65"/>
+      <c r="AF19" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG19" s="41"/>
-      <c r="AH19" s="41"/>
-      <c r="AI19" s="41"/>
-      <c r="AJ19" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK19" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL19" s="41"/>
-      <c r="AM19" s="41"/>
-      <c r="AN19" s="41"/>
-      <c r="AO19" s="41"/>
-      <c r="AP19" s="42">
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="39"/>
+      <c r="AI19" s="39"/>
+      <c r="AJ19" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK19" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL19" s="39"/>
+      <c r="AM19" s="38"/>
+      <c r="AN19" s="39"/>
+      <c r="AO19" s="39"/>
+      <c r="AP19" s="40">
         <v>2.3891699999999998E-2</v>
       </c>
-      <c r="AQ19" s="42">
+      <c r="AQ19" s="40">
         <v>0.26253700000000002</v>
       </c>
-      <c r="AR19" s="42">
+      <c r="AR19" s="40">
         <v>1.8078400000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="63" t="s">
         <v>139</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -8038,7 +9361,7 @@
       <c r="N20" s="40">
         <v>5.4854E-2</v>
       </c>
-      <c r="P20" s="61" t="s">
+      <c r="P20" s="63" t="s">
         <v>139</v>
       </c>
       <c r="Q20" s="38" t="s">
@@ -8074,7 +9397,7 @@
       <c r="AC20" s="40">
         <v>0.97633400000000004</v>
       </c>
-      <c r="AE20" s="61" t="s">
+      <c r="AE20" s="63" t="s">
         <v>139</v>
       </c>
       <c r="AF20" s="38" t="s">
@@ -8112,7 +9435,7 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="38" t="s">
         <v>133</v>
       </c>
@@ -8150,7 +9473,7 @@
       <c r="N21" s="40">
         <v>0.40772999999999998</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="64"/>
       <c r="Q21" s="38" t="s">
         <v>133</v>
       </c>
@@ -8184,7 +9507,7 @@
       <c r="AC21" s="40">
         <v>0.34917199999999998</v>
       </c>
-      <c r="AE21" s="62"/>
+      <c r="AE21" s="64"/>
       <c r="AF21" s="38" t="s">
         <v>133</v>
       </c>
@@ -8206,7 +9529,7 @@
       <c r="AL21" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="AM21" s="38" t="s">
+      <c r="AM21" s="56" t="s">
         <v>108</v>
       </c>
       <c r="AN21" s="39"/>
@@ -8222,7 +9545,7 @@
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="38" t="s">
         <v>134</v>
       </c>
@@ -8256,7 +9579,7 @@
       <c r="N22" s="40">
         <v>5.7199100000000003E-2</v>
       </c>
-      <c r="P22" s="62"/>
+      <c r="P22" s="64"/>
       <c r="Q22" s="38" t="s">
         <v>134</v>
       </c>
@@ -8290,7 +9613,7 @@
       <c r="AC22" s="40">
         <v>0.98668299999999998</v>
       </c>
-      <c r="AE22" s="62"/>
+      <c r="AE22" s="64"/>
       <c r="AF22" s="38" t="s">
         <v>134</v>
       </c>
@@ -8310,7 +9633,7 @@
         <v>108</v>
       </c>
       <c r="AL22" s="39"/>
-      <c r="AM22" s="38" t="s">
+      <c r="AM22" s="56" t="s">
         <v>108</v>
       </c>
       <c r="AN22" s="39" t="s">
@@ -8328,7 +9651,7 @@
       </c>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A23" s="63"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="41" t="s">
         <v>135</v>
       </c>
@@ -8350,7 +9673,7 @@
       <c r="N23" s="42">
         <v>7.4505699999999994E-2</v>
       </c>
-      <c r="P23" s="63"/>
+      <c r="P23" s="65"/>
       <c r="Q23" s="41" t="s">
         <v>135</v>
       </c>
@@ -8380,35 +9703,35 @@
       <c r="AC23" s="42">
         <v>0.96269300000000002</v>
       </c>
-      <c r="AE23" s="63"/>
-      <c r="AF23" s="41" t="s">
+      <c r="AE23" s="65"/>
+      <c r="AF23" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG23" s="41"/>
-      <c r="AH23" s="41"/>
-      <c r="AI23" s="41"/>
-      <c r="AJ23" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK23" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL23" s="41"/>
-      <c r="AM23" s="41"/>
-      <c r="AN23" s="41"/>
-      <c r="AO23" s="41"/>
-      <c r="AP23" s="42">
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="39"/>
+      <c r="AI23" s="39"/>
+      <c r="AJ23" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK23" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL23" s="39"/>
+      <c r="AM23" s="38"/>
+      <c r="AN23" s="39"/>
+      <c r="AO23" s="39"/>
+      <c r="AP23" s="40">
         <v>1.78631E-2</v>
       </c>
-      <c r="AQ23" s="42">
+      <c r="AQ23" s="40">
         <v>1.0533300000000001E-2</v>
       </c>
-      <c r="AR23" s="42">
+      <c r="AR23" s="40">
         <v>0.190696</v>
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="59" t="s">
         <v>140</v>
       </c>
       <c r="B24" s="38" t="s">
@@ -8450,7 +9773,7 @@
       <c r="N24" s="40">
         <v>0.25895099999999999</v>
       </c>
-      <c r="P24" s="57" t="s">
+      <c r="P24" s="59" t="s">
         <v>140</v>
       </c>
       <c r="Q24" s="38" t="s">
@@ -8486,7 +9809,7 @@
       <c r="AC24" s="40">
         <v>0.391177</v>
       </c>
-      <c r="AE24" s="57" t="s">
+      <c r="AE24" s="59" t="s">
         <v>140</v>
       </c>
       <c r="AF24" s="38" t="s">
@@ -8528,7 +9851,7 @@
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="38" t="s">
         <v>133</v>
       </c>
@@ -8562,7 +9885,7 @@
       <c r="N25" s="40">
         <v>8.7913599999999995E-2</v>
       </c>
-      <c r="P25" s="58"/>
+      <c r="P25" s="60"/>
       <c r="Q25" s="38" t="s">
         <v>133</v>
       </c>
@@ -8596,7 +9919,7 @@
       <c r="AC25" s="40">
         <v>0.992869</v>
       </c>
-      <c r="AE25" s="58"/>
+      <c r="AE25" s="60"/>
       <c r="AF25" s="38" t="s">
         <v>133</v>
       </c>
@@ -8632,7 +9955,7 @@
       </c>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="38" t="s">
         <v>134</v>
       </c>
@@ -8668,7 +9991,7 @@
       <c r="N26" s="40">
         <v>8.6047599999999999E-5</v>
       </c>
-      <c r="P26" s="58"/>
+      <c r="P26" s="60"/>
       <c r="Q26" s="38" t="s">
         <v>134</v>
       </c>
@@ -8704,7 +10027,7 @@
       <c r="AC26" s="40">
         <v>0.49700499999999997</v>
       </c>
-      <c r="AE26" s="58"/>
+      <c r="AE26" s="60"/>
       <c r="AF26" s="38" t="s">
         <v>134</v>
       </c>
@@ -8727,7 +10050,7 @@
         <v>108</v>
       </c>
       <c r="AM26" s="38"/>
-      <c r="AN26" s="39" t="s">
+      <c r="AN26" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AO26" s="39" t="s">
@@ -8744,7 +10067,7 @@
       </c>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="41" t="s">
         <v>135</v>
       </c>
@@ -8766,7 +10089,7 @@
       <c r="N27" s="42">
         <v>5.1660999999999999E-2</v>
       </c>
-      <c r="P27" s="59"/>
+      <c r="P27" s="61"/>
       <c r="Q27" s="41" t="s">
         <v>135</v>
       </c>
@@ -8794,33 +10117,33 @@
       <c r="AC27" s="42">
         <v>0.59972999999999999</v>
       </c>
-      <c r="AE27" s="59"/>
-      <c r="AF27" s="41" t="s">
+      <c r="AE27" s="61"/>
+      <c r="AF27" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG27" s="41"/>
-      <c r="AH27" s="41"/>
-      <c r="AI27" s="41"/>
-      <c r="AJ27" s="41"/>
-      <c r="AK27" s="41"/>
-      <c r="AL27" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM27" s="41"/>
-      <c r="AN27" s="41"/>
-      <c r="AO27" s="41"/>
-      <c r="AP27" s="42">
+      <c r="AG27" s="38"/>
+      <c r="AH27" s="39"/>
+      <c r="AI27" s="39"/>
+      <c r="AJ27" s="38"/>
+      <c r="AK27" s="39"/>
+      <c r="AL27" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM27" s="38"/>
+      <c r="AN27" s="39"/>
+      <c r="AO27" s="39"/>
+      <c r="AP27" s="40">
         <v>5.3174899999999997E-2</v>
       </c>
-      <c r="AQ27" s="42">
+      <c r="AQ27" s="40">
         <v>7.1961000000000004E-3</v>
       </c>
-      <c r="AR27" s="42">
+      <c r="AR27" s="40">
         <v>2.1038399999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="59" t="s">
         <v>116</v>
       </c>
       <c r="B28" s="38" t="s">
@@ -8856,7 +10179,7 @@
       <c r="N28" s="40">
         <v>0.21804599999999999</v>
       </c>
-      <c r="P28" s="57" t="s">
+      <c r="P28" s="59" t="s">
         <v>116</v>
       </c>
       <c r="Q28" s="38" t="s">
@@ -8892,27 +10215,45 @@
       <c r="AC28" s="40">
         <v>0.79758499999999999</v>
       </c>
-      <c r="AE28" s="57" t="s">
+      <c r="AE28" s="59" t="s">
         <v>116</v>
       </c>
       <c r="AF28" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG28" s="38"/>
-      <c r="AH28" s="39"/>
-      <c r="AI28" s="39"/>
-      <c r="AJ28" s="38"/>
-      <c r="AK28" s="39"/>
-      <c r="AL28" s="39"/>
+      <c r="AG28" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH28" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI28" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ28" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK28" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL28" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM28" s="38"/>
       <c r="AN28" s="39"/>
       <c r="AO28" s="39"/>
-      <c r="AP28" s="40"/>
-      <c r="AQ28" s="40"/>
-      <c r="AR28" s="40"/>
+      <c r="AP28" s="40">
+        <v>0.28936299999999998</v>
+      </c>
+      <c r="AQ28" s="40">
+        <v>0.80910199999999999</v>
+      </c>
+      <c r="AR28" s="40">
+        <v>4.2327399999999996E-3</v>
+      </c>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="38" t="s">
         <v>133</v>
       </c>
@@ -8946,7 +10287,7 @@
       <c r="N29" s="40">
         <v>1.9599700000000001E-2</v>
       </c>
-      <c r="P29" s="58"/>
+      <c r="P29" s="60"/>
       <c r="Q29" s="38" t="s">
         <v>133</v>
       </c>
@@ -8980,25 +10321,43 @@
       <c r="AC29" s="40">
         <v>0.20802399999999999</v>
       </c>
-      <c r="AE29" s="58"/>
+      <c r="AE29" s="60"/>
       <c r="AF29" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG29" s="38"/>
-      <c r="AH29" s="39"/>
-      <c r="AI29" s="39"/>
-      <c r="AJ29" s="38"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="39"/>
+      <c r="AG29" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH29" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI29" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ29" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK29" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL29" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM29" s="38"/>
       <c r="AN29" s="39"/>
       <c r="AO29" s="39"/>
-      <c r="AP29" s="40"/>
-      <c r="AQ29" s="40"/>
-      <c r="AR29" s="40"/>
+      <c r="AP29" s="40">
+        <v>0.12768599999999999</v>
+      </c>
+      <c r="AQ29" s="40">
+        <v>0.23233300000000001</v>
+      </c>
+      <c r="AR29" s="40">
+        <v>1.1742900000000001E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A30" s="58"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="38" t="s">
         <v>134</v>
       </c>
@@ -9032,7 +10391,7 @@
       <c r="N30" s="40">
         <v>7.6017100000000002E-4</v>
       </c>
-      <c r="P30" s="58"/>
+      <c r="P30" s="60"/>
       <c r="Q30" s="38" t="s">
         <v>134</v>
       </c>
@@ -9066,25 +10425,43 @@
       <c r="AC30" s="40">
         <v>0.55451899999999998</v>
       </c>
-      <c r="AE30" s="58"/>
+      <c r="AE30" s="60"/>
       <c r="AF30" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG30" s="38"/>
-      <c r="AH30" s="39"/>
-      <c r="AI30" s="39"/>
-      <c r="AJ30" s="38"/>
-      <c r="AK30" s="39"/>
-      <c r="AL30" s="39"/>
+      <c r="AG30" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH30" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI30" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ30" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK30" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL30" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM30" s="38"/>
       <c r="AN30" s="39"/>
       <c r="AO30" s="39"/>
-      <c r="AP30" s="40"/>
-      <c r="AQ30" s="40"/>
-      <c r="AR30" s="40"/>
+      <c r="AP30" s="40">
+        <v>6.3838300000000001E-2</v>
+      </c>
+      <c r="AQ30" s="40">
+        <v>0.39498299999999997</v>
+      </c>
+      <c r="AR30" s="40">
+        <v>1.8096000000000001E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="41" t="s">
         <v>135</v>
       </c>
@@ -9106,7 +10483,7 @@
       <c r="N31" s="42">
         <v>6.0392800000000003E-2</v>
       </c>
-      <c r="P31" s="59"/>
+      <c r="P31" s="61"/>
       <c r="Q31" s="41" t="s">
         <v>135</v>
       </c>
@@ -9134,25 +10511,35 @@
       <c r="AC31" s="42">
         <v>0.40330300000000002</v>
       </c>
-      <c r="AE31" s="59"/>
-      <c r="AF31" s="41" t="s">
+      <c r="AE31" s="61"/>
+      <c r="AF31" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG31" s="41"/>
-      <c r="AH31" s="41"/>
-      <c r="AI31" s="41"/>
-      <c r="AJ31" s="41"/>
-      <c r="AK31" s="41"/>
-      <c r="AL31" s="41"/>
-      <c r="AM31" s="41"/>
-      <c r="AN31" s="41"/>
-      <c r="AO31" s="41"/>
-      <c r="AP31" s="42"/>
-      <c r="AQ31" s="42"/>
-      <c r="AR31" s="42"/>
+      <c r="AG31" s="38"/>
+      <c r="AH31" s="39"/>
+      <c r="AI31" s="39"/>
+      <c r="AJ31" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK31" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL31" s="39"/>
+      <c r="AM31" s="38"/>
+      <c r="AN31" s="39"/>
+      <c r="AO31" s="39"/>
+      <c r="AP31" s="40">
+        <v>7.8202800000000003E-2</v>
+      </c>
+      <c r="AQ31" s="40">
+        <v>7.1798000000000001E-2</v>
+      </c>
+      <c r="AR31" s="40">
+        <v>2.3383000000000001E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="59" t="s">
         <v>141</v>
       </c>
       <c r="B32" s="38" t="s">
@@ -9192,7 +10579,7 @@
       <c r="N32" s="40">
         <v>6.8416699999999997E-2</v>
       </c>
-      <c r="P32" s="57" t="s">
+      <c r="P32" s="59" t="s">
         <v>141</v>
       </c>
       <c r="Q32" s="38" t="s">
@@ -9228,27 +10615,49 @@
       <c r="AC32" s="40">
         <v>0.79306100000000002</v>
       </c>
-      <c r="AE32" s="57" t="s">
+      <c r="AE32" s="59" t="s">
         <v>141</v>
       </c>
       <c r="AF32" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG32" s="38"/>
-      <c r="AH32" s="39"/>
-      <c r="AI32" s="39"/>
-      <c r="AJ32" s="38"/>
-      <c r="AK32" s="39"/>
-      <c r="AL32" s="39"/>
-      <c r="AM32" s="38"/>
+      <c r="AG32" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ32" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM32" s="56" t="s">
+        <v>108</v>
+      </c>
       <c r="AN32" s="39"/>
-      <c r="AO32" s="39"/>
-      <c r="AP32" s="40"/>
-      <c r="AQ32" s="40"/>
-      <c r="AR32" s="40"/>
+      <c r="AO32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP32" s="40">
+        <v>0.14907400000000001</v>
+      </c>
+      <c r="AQ32" s="40">
+        <v>3.2127000000000003E-2</v>
+      </c>
+      <c r="AR32" s="40">
+        <v>2.40463E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="38" t="s">
         <v>133</v>
       </c>
@@ -9282,7 +10691,7 @@
       <c r="N33" s="40">
         <v>0.24232799999999999</v>
       </c>
-      <c r="P33" s="58"/>
+      <c r="P33" s="60"/>
       <c r="Q33" s="38" t="s">
         <v>133</v>
       </c>
@@ -9316,25 +10725,43 @@
       <c r="AC33" s="40">
         <v>0.79171599999999998</v>
       </c>
-      <c r="AE33" s="58"/>
+      <c r="AE33" s="60"/>
       <c r="AF33" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG33" s="38"/>
-      <c r="AH33" s="39"/>
-      <c r="AI33" s="39"/>
-      <c r="AJ33" s="38"/>
-      <c r="AK33" s="39"/>
-      <c r="AL33" s="39"/>
+      <c r="AG33" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH33" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI33" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ33" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK33" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL33" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM33" s="38"/>
       <c r="AN33" s="39"/>
       <c r="AO33" s="39"/>
-      <c r="AP33" s="40"/>
-      <c r="AQ33" s="40"/>
-      <c r="AR33" s="40"/>
+      <c r="AP33" s="40">
+        <v>0.42867</v>
+      </c>
+      <c r="AQ33" s="40">
+        <v>8.9202199999999995E-2</v>
+      </c>
+      <c r="AR33" s="40">
+        <v>0.12592999999999999</v>
+      </c>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A34" s="58"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="38" t="s">
         <v>134</v>
       </c>
@@ -9368,7 +10795,7 @@
       <c r="N34" s="40">
         <v>9.2139299999999993E-2</v>
       </c>
-      <c r="P34" s="58"/>
+      <c r="P34" s="60"/>
       <c r="Q34" s="38" t="s">
         <v>134</v>
       </c>
@@ -9404,25 +10831,47 @@
       <c r="AC34" s="40">
         <v>5.10708E-2</v>
       </c>
-      <c r="AE34" s="58"/>
+      <c r="AE34" s="60"/>
       <c r="AF34" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG34" s="38"/>
-      <c r="AH34" s="39"/>
-      <c r="AI34" s="39"/>
-      <c r="AJ34" s="38"/>
-      <c r="AK34" s="39"/>
-      <c r="AL34" s="39"/>
-      <c r="AM34" s="38"/>
+      <c r="AG34" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH34" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI34" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ34" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK34" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL34" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM34" s="56" t="s">
+        <v>108</v>
+      </c>
       <c r="AN34" s="39"/>
-      <c r="AO34" s="39"/>
-      <c r="AP34" s="40"/>
-      <c r="AQ34" s="40"/>
-      <c r="AR34" s="40"/>
+      <c r="AO34" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP34" s="40">
+        <v>0.36803900000000001</v>
+      </c>
+      <c r="AQ34" s="40">
+        <v>7.62462E-2</v>
+      </c>
+      <c r="AR34" s="40">
+        <v>3.55566E-3</v>
+      </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="41" t="s">
         <v>135</v>
       </c>
@@ -9444,7 +10893,7 @@
       <c r="N35" s="42">
         <v>3.5705899999999999E-2</v>
       </c>
-      <c r="P35" s="59"/>
+      <c r="P35" s="61"/>
       <c r="Q35" s="41" t="s">
         <v>135</v>
       </c>
@@ -9476,25 +10925,41 @@
       <c r="AC35" s="42">
         <v>0.37054599999999999</v>
       </c>
-      <c r="AE35" s="59"/>
-      <c r="AF35" s="41" t="s">
+      <c r="AE35" s="61"/>
+      <c r="AF35" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG35" s="41"/>
-      <c r="AH35" s="41"/>
-      <c r="AI35" s="41"/>
-      <c r="AJ35" s="41"/>
-      <c r="AK35" s="41"/>
-      <c r="AL35" s="41"/>
-      <c r="AM35" s="41"/>
-      <c r="AN35" s="41"/>
-      <c r="AO35" s="41"/>
-      <c r="AP35" s="42"/>
-      <c r="AQ35" s="42"/>
-      <c r="AR35" s="42"/>
+      <c r="AG35" s="38"/>
+      <c r="AH35" s="39"/>
+      <c r="AI35" s="39"/>
+      <c r="AJ35" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK35" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL35" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM35" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN35" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO35" s="39"/>
+      <c r="AP35" s="40">
+        <v>3.6327900000000003E-2</v>
+      </c>
+      <c r="AQ35" s="40">
+        <v>0.111786</v>
+      </c>
+      <c r="AR35" s="40">
+        <v>1.11094E-2</v>
+      </c>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="62" t="s">
         <v>142</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -9536,7 +11001,7 @@
       <c r="N36" s="40">
         <v>0.79885600000000001</v>
       </c>
-      <c r="P36" s="60" t="s">
+      <c r="P36" s="62" t="s">
         <v>142</v>
       </c>
       <c r="Q36" s="38" t="s">
@@ -9572,27 +11037,51 @@
       <c r="AC36" s="40">
         <v>0.119131</v>
       </c>
-      <c r="AE36" s="60" t="s">
+      <c r="AE36" s="62" t="s">
         <v>142</v>
       </c>
       <c r="AF36" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AG36" s="38"/>
-      <c r="AH36" s="39"/>
-      <c r="AI36" s="39"/>
-      <c r="AJ36" s="38"/>
-      <c r="AK36" s="39"/>
-      <c r="AL36" s="39"/>
-      <c r="AM36" s="38"/>
-      <c r="AN36" s="39"/>
-      <c r="AO36" s="39"/>
-      <c r="AP36" s="40"/>
-      <c r="AQ36" s="40"/>
-      <c r="AR36" s="40"/>
+      <c r="AG36" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ36" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM36" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP36" s="40">
+        <v>1.91909E-3</v>
+      </c>
+      <c r="AQ36" s="40">
+        <v>2.6462300000000001E-2</v>
+      </c>
+      <c r="AR36" s="40">
+        <v>0.16523299999999999</v>
+      </c>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="38" t="s">
         <v>133</v>
       </c>
@@ -9626,7 +11115,7 @@
       <c r="N37" s="40">
         <v>0.51789499999999999</v>
       </c>
-      <c r="P37" s="60"/>
+      <c r="P37" s="62"/>
       <c r="Q37" s="38" t="s">
         <v>133</v>
       </c>
@@ -9660,25 +11149,43 @@
       <c r="AC37" s="40">
         <v>0.74060099999999995</v>
       </c>
-      <c r="AE37" s="60"/>
+      <c r="AE37" s="62"/>
       <c r="AF37" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="AG37" s="38"/>
-      <c r="AH37" s="39"/>
-      <c r="AI37" s="39"/>
-      <c r="AJ37" s="38"/>
-      <c r="AK37" s="39"/>
-      <c r="AL37" s="39"/>
+      <c r="AG37" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH37" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI37" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ37" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK37" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL37" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="AM37" s="38"/>
       <c r="AN37" s="39"/>
       <c r="AO37" s="39"/>
-      <c r="AP37" s="40"/>
-      <c r="AQ37" s="40"/>
-      <c r="AR37" s="40"/>
+      <c r="AP37" s="40">
+        <v>0.12167699999999999</v>
+      </c>
+      <c r="AQ37" s="40">
+        <v>0.34179199999999998</v>
+      </c>
+      <c r="AR37" s="40">
+        <v>0.30942399999999998</v>
+      </c>
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A38" s="60"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="38" t="s">
         <v>134</v>
       </c>
@@ -9700,13 +11207,13 @@
       <c r="H38" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="J38" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="K38" s="84" t="s">
+      <c r="I38" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="K38" s="39" t="s">
         <v>108</v>
       </c>
       <c r="L38" s="40">
@@ -9718,7 +11225,7 @@
       <c r="N38" s="40">
         <v>1.3228699999999999E-2</v>
       </c>
-      <c r="P38" s="60"/>
+      <c r="P38" s="62"/>
       <c r="Q38" s="38" t="s">
         <v>134</v>
       </c>
@@ -9740,13 +11247,13 @@
       <c r="W38" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="X38" s="83" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y38" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z38" s="84" t="s">
+      <c r="X38" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y38" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z38" s="57" t="s">
         <v>108</v>
       </c>
       <c r="AA38" s="40">
@@ -9758,25 +11265,49 @@
       <c r="AC38" s="40">
         <v>0.59381899999999999</v>
       </c>
-      <c r="AE38" s="60"/>
+      <c r="AE38" s="62"/>
       <c r="AF38" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="AG38" s="38"/>
-      <c r="AH38" s="39"/>
-      <c r="AI38" s="39"/>
-      <c r="AJ38" s="38"/>
-      <c r="AK38" s="39"/>
-      <c r="AL38" s="39"/>
-      <c r="AM38" s="38"/>
-      <c r="AN38" s="39"/>
-      <c r="AO38" s="39"/>
-      <c r="AP38" s="40"/>
-      <c r="AQ38" s="40"/>
-      <c r="AR38" s="40"/>
+      <c r="AG38" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ38" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM38" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN38" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP38" s="40">
+        <v>0.147316</v>
+      </c>
+      <c r="AQ38" s="40">
+        <v>0.24088399999999999</v>
+      </c>
+      <c r="AR38" s="40">
+        <v>4.1844199999999998E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A39" s="60"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="41" t="s">
         <v>135</v>
       </c>
@@ -9798,7 +11329,7 @@
       <c r="N39" s="42">
         <v>0.12786700000000001</v>
       </c>
-      <c r="P39" s="60"/>
+      <c r="P39" s="62"/>
       <c r="Q39" s="41" t="s">
         <v>135</v>
       </c>
@@ -9832,22 +11363,34 @@
       <c r="AC39" s="42">
         <v>0.94489999999999996</v>
       </c>
-      <c r="AE39" s="60"/>
-      <c r="AF39" s="41" t="s">
+      <c r="AE39" s="62"/>
+      <c r="AF39" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="AG39" s="41"/>
-      <c r="AH39" s="41"/>
-      <c r="AI39" s="41"/>
-      <c r="AJ39" s="41"/>
-      <c r="AK39" s="41"/>
-      <c r="AL39" s="41"/>
-      <c r="AM39" s="41"/>
-      <c r="AN39" s="41"/>
-      <c r="AO39" s="41"/>
-      <c r="AP39" s="42"/>
-      <c r="AQ39" s="42"/>
-      <c r="AR39" s="42"/>
+      <c r="AG39" s="38"/>
+      <c r="AH39" s="39"/>
+      <c r="AI39" s="39"/>
+      <c r="AJ39" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK39" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL39" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM39" s="38"/>
+      <c r="AN39" s="39"/>
+      <c r="AO39" s="39"/>
+      <c r="AP39" s="40">
+        <v>4.3738800000000001E-2</v>
+      </c>
+      <c r="AQ39" s="40">
+        <v>3.2079400000000001E-2</v>
+      </c>
+      <c r="AR39" s="40">
+        <v>3.1233299999999999E-2</v>
+      </c>
     </row>
     <row r="40" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
@@ -12029,36 +13572,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="64" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="64" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="69" t="s">
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="71"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="73"/>
     </row>
     <row r="2" spans="1:17" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="36" t="s">
         <v>125</v>
       </c>
@@ -12098,7 +13641,7 @@
       <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>136</v>
       </c>
       <c r="B3" s="38" t="s">
@@ -12139,7 +13682,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="38" t="s">
         <v>133</v>
       </c>
@@ -12181,7 +13724,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="38" t="s">
         <v>134</v>
       </c>
@@ -12217,7 +13760,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="41" t="s">
         <v>135</v>
       </c>
@@ -12250,7 +13793,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="59" t="s">
         <v>137</v>
       </c>
       <c r="B7" s="38" t="s">
@@ -12288,7 +13831,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="38" t="s">
         <v>133</v>
       </c>
@@ -12330,7 +13873,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="38" t="s">
         <v>134</v>
       </c>
@@ -12366,7 +13909,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="41" t="s">
         <v>135</v>
       </c>
@@ -12396,7 +13939,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="59" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="38" t="s">
@@ -12434,7 +13977,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="38" t="s">
         <v>133</v>
       </c>
@@ -12470,7 +14013,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="38" t="s">
         <v>134</v>
       </c>
@@ -12506,7 +14049,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="41" t="s">
         <v>135</v>
       </c>
@@ -12536,7 +14079,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="63" t="s">
         <v>138</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -12578,7 +14121,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="39" t="s">
         <v>133</v>
       </c>
@@ -12617,7 +14160,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="38" t="s">
         <v>134</v>
       </c>
@@ -12653,7 +14196,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="41" t="s">
         <v>135</v>
       </c>
@@ -12685,7 +14228,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="63" t="s">
         <v>139</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -12723,7 +14266,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="38" t="s">
         <v>133</v>
       </c>
@@ -12759,7 +14302,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="38" t="s">
         <v>134</v>
       </c>
@@ -12795,7 +14338,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="63"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="41" t="s">
         <v>135</v>
       </c>
@@ -12827,7 +14370,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="59" t="s">
         <v>140</v>
       </c>
       <c r="B23" s="38" t="s">
@@ -12865,7 +14408,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="38" t="s">
         <v>133</v>
       </c>
@@ -12901,7 +14444,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="38" t="s">
         <v>134</v>
       </c>
@@ -12939,7 +14482,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="41" t="s">
         <v>135</v>
       </c>
@@ -12969,7 +14512,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="59" t="s">
         <v>116</v>
       </c>
       <c r="B27" s="38" t="s">
@@ -13007,7 +14550,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="38" t="s">
         <v>133</v>
       </c>
@@ -13043,7 +14586,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="38" t="s">
         <v>134</v>
       </c>
@@ -13079,7 +14622,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="41" t="s">
         <v>135</v>
       </c>
@@ -13109,7 +14652,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="59" t="s">
         <v>141</v>
       </c>
       <c r="B31" s="38" t="s">
@@ -13147,7 +14690,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="58"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="38" t="s">
         <v>133</v>
       </c>
@@ -13183,7 +14726,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="38" t="s">
         <v>134</v>
       </c>
@@ -13221,7 +14764,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="41" t="s">
         <v>135</v>
       </c>
@@ -13255,7 +14798,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="62" t="s">
         <v>142</v>
       </c>
       <c r="B35" s="38" t="s">
@@ -13293,7 +14836,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="60"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="38" t="s">
         <v>133</v>
       </c>
@@ -13329,7 +14872,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="38" t="s">
         <v>134</v>
       </c>
@@ -13371,7 +14914,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="60"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="41" t="s">
         <v>135</v>
       </c>
@@ -14770,7 +16313,7 @@
       <c r="AT1" s="1"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="75" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -14788,7 +16331,7 @@
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="27" t="s">
         <v>109</v>
       </c>
@@ -14804,7 +16347,7 @@
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="27" t="s">
         <v>111</v>
       </c>
@@ -14820,7 +16363,7 @@
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="27" t="s">
         <v>112</v>
       </c>
@@ -14832,7 +16375,7 @@
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="78" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -14850,7 +16393,7 @@
       </c>
     </row>
     <row r="7" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="21" t="s">
         <v>109</v>
       </c>
@@ -14866,7 +16409,7 @@
       </c>
     </row>
     <row r="8" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="21" t="s">
         <v>111</v>
       </c>
@@ -14884,7 +16427,7 @@
       </c>
     </row>
     <row r="9" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
+      <c r="A9" s="80"/>
       <c r="B9" s="21" t="s">
         <v>112</v>
       </c>
@@ -14896,7 +16439,7 @@
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="75" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="27" t="s">
@@ -14914,7 +16457,7 @@
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="27" t="s">
         <v>109</v>
       </c>
@@ -14932,7 +16475,7 @@
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="27" t="s">
         <v>111</v>
       </c>
@@ -14948,7 +16491,7 @@
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="27" t="s">
         <v>112</v>
       </c>
@@ -14960,7 +16503,7 @@
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="75" t="s">
         <v>115</v>
       </c>
       <c r="B14" s="27" t="s">
@@ -14980,7 +16523,7 @@
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="27" t="s">
         <v>109</v>
       </c>
@@ -14996,7 +16539,7 @@
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="27" t="s">
         <v>111</v>
       </c>
@@ -15014,7 +16557,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="27" t="s">
         <v>112</v>
       </c>
@@ -15026,7 +16569,7 @@
       <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="75" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -15044,7 +16587,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="27" t="s">
         <v>109</v>
       </c>
@@ -15060,7 +16603,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="27" t="s">
         <v>111</v>
       </c>
@@ -15076,7 +16619,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="27" t="s">
         <v>112</v>
       </c>
@@ -15088,7 +16631,7 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="75" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="27" t="s">
@@ -15108,7 +16651,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="27" t="s">
         <v>109</v>
       </c>
@@ -15125,7 +16668,7 @@
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="27" t="s">
         <v>111</v>
       </c>
@@ -15141,7 +16684,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="27" t="s">
         <v>112</v>
       </c>
@@ -15153,7 +16696,7 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="74" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="27" t="s">
@@ -15173,7 +16716,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="27" t="s">
         <v>109</v>
       </c>
@@ -15189,7 +16732,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="72"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="27" t="s">
         <v>111</v>
       </c>
@@ -15207,7 +16750,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="27" t="s">
         <v>112</v>
       </c>
@@ -16170,7 +17713,7 @@
       <c r="AT1" s="1"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="75" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -16188,7 +17731,7 @@
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="27" t="s">
         <v>109</v>
       </c>
@@ -16204,7 +17747,7 @@
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="27" t="s">
         <v>111</v>
       </c>
@@ -16220,7 +17763,7 @@
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="27" t="s">
         <v>112</v>
       </c>
@@ -16232,7 +17775,7 @@
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="78" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -16250,7 +17793,7 @@
       </c>
     </row>
     <row r="7" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="21" t="s">
         <v>109</v>
       </c>
@@ -16266,7 +17809,7 @@
       </c>
     </row>
     <row r="8" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="21" t="s">
         <v>111</v>
       </c>
@@ -16282,7 +17825,7 @@
       </c>
     </row>
     <row r="9" spans="1:46" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
+      <c r="A9" s="80"/>
       <c r="B9" s="21" t="s">
         <v>112</v>
       </c>
@@ -16294,7 +17837,7 @@
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="75" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="27" t="s">
@@ -16312,7 +17855,7 @@
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="27" t="s">
         <v>109</v>
       </c>
@@ -16328,7 +17871,7 @@
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="27" t="s">
         <v>111</v>
       </c>
@@ -16344,7 +17887,7 @@
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="27" t="s">
         <v>112</v>
       </c>
@@ -16356,7 +17899,7 @@
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="75" t="s">
         <v>115</v>
       </c>
       <c r="B14" s="27" t="s">
@@ -16376,7 +17919,7 @@
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="27" t="s">
         <v>109</v>
       </c>
@@ -16392,7 +17935,7 @@
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="27" t="s">
         <v>111</v>
       </c>
@@ -16408,7 +17951,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="27" t="s">
         <v>112</v>
       </c>
@@ -16420,7 +17963,7 @@
       <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="75" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -16438,7 +17981,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="27" t="s">
         <v>109</v>
       </c>
@@ -16454,7 +17997,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="27" t="s">
         <v>111</v>
       </c>
@@ -16470,7 +18013,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="27" t="s">
         <v>112</v>
       </c>
@@ -16482,7 +18025,7 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="75" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="27" t="s">
@@ -16502,7 +18045,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="27" t="s">
         <v>109</v>
       </c>
@@ -16519,7 +18062,7 @@
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="27" t="s">
         <v>111</v>
       </c>
@@ -16535,7 +18078,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="27" t="s">
         <v>112</v>
       </c>
@@ -16547,7 +18090,7 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="74" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="27" t="s">
@@ -16567,7 +18110,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="27" t="s">
         <v>109</v>
       </c>
@@ -16583,7 +18126,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="72"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="27" t="s">
         <v>111</v>
       </c>
@@ -16601,7 +18144,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="27" t="s">
         <v>112</v>
       </c>
@@ -17501,18 +19044,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81"/>
-      <c r="H1" s="79" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
+      <c r="H1" s="81" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="81"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="83"/>
     </row>
     <row r="2" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
@@ -19085,18 +20628,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="F1" s="82" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="F1" s="84" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">

</xml_diff>